<commit_message>
Removed processing of optional/suggested profile items. General output cleanup. More updates to example profile
</commit_message>
<xml_diff>
--- a/examples/Example_Profile.xlsx
+++ b/examples/Example_Profile.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="87">
   <si>
     <t>Profile Information</t>
   </si>
@@ -223,6 +223,63 @@
   </si>
   <si>
     <t>Instance Selectors</t>
+  </si>
+  <si>
+    <t>TTPsType</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>stix:STIX_Package/stix:TTPs</t>
+  </si>
+  <si>
+    <t>stix:STIXHeaderType</t>
+  </si>
+  <si>
+    <t>cybox:ObservablesType</t>
+  </si>
+  <si>
+    <t>stix:IndicatorsType</t>
+  </si>
+  <si>
+    <t>stix:TTPsType</t>
+  </si>
+  <si>
+    <t>stixCommon:ExploitTargetsType</t>
+  </si>
+  <si>
+    <t>stix:IncidentsType</t>
+  </si>
+  <si>
+    <t>stix:CoursesOfActionType</t>
+  </si>
+  <si>
+    <t>stix:CampaignsType</t>
+  </si>
+  <si>
+    <t>stix:ThreatActorsType</t>
+  </si>
+  <si>
+    <t>xs:QName</t>
+  </si>
+  <si>
+    <t>stix:STIXPackageVersionEnum</t>
+  </si>
+  <si>
+    <t>xs:string</t>
+  </si>
+  <si>
+    <t>stixCommon:ControlledVocabularyStringType</t>
+  </si>
+  <si>
+    <t>stixCommon:StructuredTextType</t>
+  </si>
+  <si>
+    <t>marking:MarkingType</t>
+  </si>
+  <si>
+    <t>stixCommon:InformationSourceType</t>
   </si>
 </sst>
 </file>
@@ -303,13 +360,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
       <sz val="15"/>
       <color rgb="FF1F497D"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -341,8 +399,9 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -390,7 +449,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -418,12 +477,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF000000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -560,15 +613,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thick">
@@ -577,13 +621,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -606,34 +659,33 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="14" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" xfId="2" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="26" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="27" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="13" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Good" xfId="2" builtinId="26"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -943,223 +995,223 @@
   <sheetFormatPr defaultColWidth="10.109375" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="67.6640625" customWidth="1"/>
-    <col min="2" max="2" width="34.5546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.5546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.6640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.5546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.5546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.6640625" style="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
     </row>
     <row r="2" spans="1:6" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
     </row>
     <row r="3" spans="1:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
     </row>
     <row r="5" spans="1:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
     </row>
     <row r="6" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
     </row>
     <row r="7" spans="1:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="28" t="s">
+      <c r="D7" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
     </row>
     <row r="8" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="D8" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
     </row>
     <row r="9" spans="1:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A9" s="10"/>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="29" t="s">
+      <c r="D9" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
     </row>
     <row r="10" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="16"/>
-      <c r="B10" s="24" t="s">
+      <c r="A10" s="15"/>
+      <c r="B10" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="27" t="s">
+      <c r="D10" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
     </row>
     <row r="11" spans="1:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="16"/>
-      <c r="B11" s="23" t="s">
+      <c r="A11" s="15"/>
+      <c r="B11" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="D11" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
     </row>
     <row r="12" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
+      <c r="A12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
     </row>
     <row r="13" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
+      <c r="A13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
     </row>
     <row r="14" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
+      <c r="A14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
     </row>
     <row r="15" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
+      <c r="A15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
     </row>
     <row r="16" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
+      <c r="A16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
     </row>
     <row r="17" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
+      <c r="A17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
     </row>
     <row r="18" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
+      <c r="A18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
     </row>
     <row r="19" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
+      <c r="A19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
     </row>
     <row r="20" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
+      <c r="A20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1168,218 +1220,273 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.109375" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="57.5546875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="66.6640625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="46.33203125" style="11" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" style="11" customWidth="1"/>
-    <col min="5" max="5" width="9.44140625" style="11"/>
+    <col min="2" max="2" width="14.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.33203125" style="11" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" style="11" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="13" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" s="13" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="16"/>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F1" s="15"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="16"/>
-    </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
+      <c r="B2" s="17"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="15"/>
+    </row>
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-    </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+    </row>
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-    </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
+      <c r="C4" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+    </row>
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-    </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="C5" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+    </row>
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-    </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+    </row>
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-    </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+    </row>
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-    </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+    </row>
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-    </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+    </row>
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-    </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+    </row>
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-    </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="14" t="s">
+      <c r="C11" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+    </row>
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-    </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+    </row>
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-    </row>
-    <row r="14" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="14" t="s">
+      <c r="C13" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+    </row>
+    <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="11" t="s">
+      <c r="C14" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="D14" s="15"/>
+      <c r="E14" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="16"/>
-    </row>
-    <row r="15" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="16"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-    </row>
-    <row r="16" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A16" s="16"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-    </row>
-    <row r="17" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="16"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-    </row>
-    <row r="18" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A18" s="16"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-    </row>
-    <row r="19" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A19" s="16"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-    </row>
-    <row r="20" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A20" s="16"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
+      <c r="F14" s="15"/>
+    </row>
+    <row r="15" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+    </row>
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="18"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+    </row>
+    <row r="17" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+    </row>
+    <row r="18" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A18" s="15"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+    </row>
+    <row r="19" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A19" s="15"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+    </row>
+    <row r="20" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A20" s="15"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1388,194 +1495,227 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.109375" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="57.5546875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="17.44140625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="78" style="11" customWidth="1"/>
-    <col min="4" max="4" width="21.5546875" style="11" customWidth="1"/>
-    <col min="5" max="5" width="9.44140625" style="11"/>
+    <col min="2" max="2" width="14.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.21875" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="78" style="11" customWidth="1"/>
+    <col min="5" max="5" width="21.5546875" style="11" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="13" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" s="13" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="16"/>
-    </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F1" s="15"/>
+    </row>
+    <row r="2" spans="1:6" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="16"/>
-    </row>
-    <row r="3" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="15"/>
+    </row>
+    <row r="3" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-    </row>
-    <row r="4" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
+      <c r="C3" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+    </row>
+    <row r="4" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="E4" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="16"/>
-    </row>
-    <row r="5" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="F4" s="15"/>
+    </row>
+    <row r="5" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-    </row>
-    <row r="6" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
+      <c r="C5" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+    </row>
+    <row r="6" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-    </row>
-    <row r="7" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="s">
+      <c r="C6" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+    </row>
+    <row r="7" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-    </row>
-    <row r="8" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-    </row>
-    <row r="9" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-    </row>
-    <row r="10" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-    </row>
-    <row r="11" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="16"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-    </row>
-    <row r="12" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="16"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-    </row>
-    <row r="13" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A13" s="16"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-    </row>
-    <row r="14" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="16"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-    </row>
-    <row r="15" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="16"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-    </row>
-    <row r="16" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A16" s="16"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-    </row>
-    <row r="17" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="16"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-    </row>
-    <row r="18" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A18" s="16"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-    </row>
-    <row r="19" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A19" s="16"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-    </row>
-    <row r="20" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A20" s="16"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
+      <c r="C7" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+    </row>
+    <row r="8" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+    </row>
+    <row r="9" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+    </row>
+    <row r="10" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+    </row>
+    <row r="11" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+    </row>
+    <row r="12" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+    </row>
+    <row r="13" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+    </row>
+    <row r="14" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+    </row>
+    <row r="15" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A15" s="15"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+    </row>
+    <row r="16" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+    </row>
+    <row r="17" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+    </row>
+    <row r="18" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A18" s="15"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+    </row>
+    <row r="19" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A19" s="15"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+    </row>
+    <row r="20" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A20" s="15"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1584,55 +1724,60 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.109375" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="57.5546875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="66.6640625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="46.33203125" style="11" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" style="11" customWidth="1"/>
-    <col min="5" max="5" width="9.44140625" style="11"/>
+    <col min="2" max="2" width="14.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.33203125" style="11" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" style="11" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="13" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" s="13" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="16"/>
-    </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F1" s="15"/>
+    </row>
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="16"/>
-    </row>
-    <row r="3" spans="1:5" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="19" t="s">
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="15"/>
+    </row>
+    <row r="3" spans="1:6" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
+      <c r="C3" s="20" t="s">
+        <v>82</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1644,14 +1789,14 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.88671875" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.88671875" customWidth="1"/>
     <col min="2" max="2" width="27.88671875" customWidth="1"/>
-    <col min="3" max="4" width="9.88671875" style="22"/>
+    <col min="3" max="4" width="9.88671875" style="20"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="13" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -1661,151 +1806,151 @@
       <c r="B1" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="16"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="15"/>
     </row>
     <row r="2" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="str">
+      <c r="A2" s="14" t="str">
         <f>HYPERLINK("http://www.w3.org/2001/XMLSchema-instance","http://www.w3.org/2001/XMLSchema-instance")</f>
         <v>http://www.w3.org/2001/XMLSchema-instance</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
     </row>
     <row r="3" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="str">
+      <c r="A3" s="14" t="str">
         <f>HYPERLINK("http://stix.mitre.org/stix-1","http://stix.mitre.org/stix-1")</f>
         <v>http://stix.mitre.org/stix-1</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="15" t="str">
+      <c r="A4" s="14" t="str">
         <f>HYPERLINK("http://stix.mitre.org/common-1","http://stix.mitre.org/common-1")</f>
         <v>http://stix.mitre.org/common-1</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
     </row>
     <row r="5" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="15" t="str">
+      <c r="A5" s="14" t="str">
         <f>HYPERLINK("http://stix.mitre.org/default_vocabularies-1","http://stix.mitre.org/default_vocabularies-1")</f>
         <v>http://stix.mitre.org/default_vocabularies-1</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
     </row>
     <row r="6" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
     </row>
     <row r="7" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
     </row>
     <row r="8" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
     </row>
     <row r="9" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
     </row>
     <row r="10" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
     </row>
     <row r="11" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="16"/>
-      <c r="B11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
     </row>
     <row r="12" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="16"/>
-      <c r="B12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
     </row>
     <row r="13" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A13" s="16"/>
-      <c r="B13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
     </row>
     <row r="14" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="16"/>
-      <c r="B14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
     </row>
     <row r="15" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="16"/>
-      <c r="B15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
+      <c r="A15" s="15"/>
+      <c r="B15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
     </row>
     <row r="16" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A16" s="16"/>
-      <c r="B16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
     </row>
     <row r="17" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="16"/>
-      <c r="B17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
     </row>
     <row r="18" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A18" s="16"/>
-      <c r="B18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
+      <c r="A18" s="15"/>
+      <c r="B18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
     </row>
     <row r="19" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A19" s="16"/>
-      <c r="B19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
+      <c r="A19" s="15"/>
+      <c r="B19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
     </row>
     <row r="20" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A20" s="16"/>
-      <c r="B20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
+      <c r="A20" s="15"/>
+      <c r="B20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1818,29 +1963,29 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.88671875" customWidth="1"/>
     <col min="2" max="2" width="100" customWidth="1"/>
-    <col min="3" max="4" width="17.109375" style="22"/>
+    <col min="3" max="4" width="17.109375" style="20"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="13" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="16"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="15"/>
     </row>
     <row r="2" spans="1:5" ht="12.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1862,8 +2007,16 @@
       <c r="A4" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="20" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated example to demonstrate disallowed CybOX Object types
</commit_message>
<xml_diff>
--- a/examples/Example_Profile.xlsx
+++ b/examples/Example_Profile.xlsx
@@ -11,15 +11,16 @@
     <sheet name="STIX Package" sheetId="2" r:id="rId2"/>
     <sheet name="STIX Header" sheetId="3" r:id="rId3"/>
     <sheet name="TTP" sheetId="4" r:id="rId4"/>
-    <sheet name="Namespaces" sheetId="5" r:id="rId5"/>
-    <sheet name="Instance Mapping" sheetId="6" r:id="rId6"/>
+    <sheet name="Indicator" sheetId="7" r:id="rId5"/>
+    <sheet name="Namespaces" sheetId="5" r:id="rId6"/>
+    <sheet name="Instance Mapping" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="207">
   <si>
     <t>Profile Information</t>
   </si>
@@ -280,13 +281,373 @@
   </si>
   <si>
     <t>stixCommon:InformationSourceType</t>
+  </si>
+  <si>
+    <t>stixCommon:TTPBaseType</t>
+  </si>
+  <si>
+    <t>Indicator</t>
+  </si>
+  <si>
+    <t>Observable</t>
+  </si>
+  <si>
+    <t>Course of Action</t>
+  </si>
+  <si>
+    <t>Incident</t>
+  </si>
+  <si>
+    <t>Exploit Target</t>
+  </si>
+  <si>
+    <t>Threat Actor</t>
+  </si>
+  <si>
+    <t>Campaign</t>
+  </si>
+  <si>
+    <t xml:space="preserve">API Object </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Account Object </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address Object </t>
+  </si>
+  <si>
+    <t>Artifact Object</t>
+  </si>
+  <si>
+    <t>Code Object</t>
+  </si>
+  <si>
+    <t>Custom Object</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DNS Cache Object </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DNS Query Object </t>
+  </si>
+  <si>
+    <t>DNS Record Object</t>
+  </si>
+  <si>
+    <t>Device Object</t>
+  </si>
+  <si>
+    <t>Disk Object</t>
+  </si>
+  <si>
+    <t>Disk Partition Object</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email Message Object </t>
+  </si>
+  <si>
+    <t>File Object</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GUI Dialogbox Object </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GUI Object </t>
+  </si>
+  <si>
+    <t>GUI Window Object</t>
+  </si>
+  <si>
+    <t>HTTP Session Object</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Library Object </t>
+  </si>
+  <si>
+    <t>Link Object</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linux Package Object </t>
+  </si>
+  <si>
+    <t>Memory Object</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mutex Object </t>
+  </si>
+  <si>
+    <t>Network Connection Object</t>
+  </si>
+  <si>
+    <t>Network Flow Object</t>
+  </si>
+  <si>
+    <t>Network Packet Object</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Network Route Entry Object </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Network Route Object </t>
+  </si>
+  <si>
+    <t>Network Socket Object</t>
+  </si>
+  <si>
+    <t>Network Subnet Object</t>
+  </si>
+  <si>
+    <t>PDF File Object 1.0 XSD HTML</t>
+  </si>
+  <si>
+    <t>Pipe Object</t>
+  </si>
+  <si>
+    <t>Port Object</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Process Object </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product Object </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Semaphore Object </t>
+  </si>
+  <si>
+    <t>Socket Address Object</t>
+  </si>
+  <si>
+    <t>System Object</t>
+  </si>
+  <si>
+    <t xml:space="preserve">URI Object </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unix File Object </t>
+  </si>
+  <si>
+    <t>Unix Network Route Entry Object</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unix Pipe Object </t>
+  </si>
+  <si>
+    <t>Unix Process Object</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unix User Account Object </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unix Volume Object </t>
+  </si>
+  <si>
+    <t>User Account Object</t>
+  </si>
+  <si>
+    <t>User Session Object</t>
+  </si>
+  <si>
+    <t>Volume Object</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whois Object </t>
+  </si>
+  <si>
+    <t>Win Computer Account Object</t>
+  </si>
+  <si>
+    <t>Win Critical Section Object</t>
+  </si>
+  <si>
+    <t>Win Driver Object</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Win Event Log Object </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Win Event Object </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Win Executable File Object </t>
+  </si>
+  <si>
+    <t>Win File Object</t>
+  </si>
+  <si>
+    <t>Win Handle Object</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Win Kernel Hook Object </t>
+  </si>
+  <si>
+    <t>Win Kernel Object</t>
+  </si>
+  <si>
+    <t>Win Mailslot Object</t>
+  </si>
+  <si>
+    <t>Win Memory Page Region Object</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Win Mutex Object </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Win Network Route Entry Object </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Win Network Share Object </t>
+  </si>
+  <si>
+    <t>Win Pipe Object</t>
+  </si>
+  <si>
+    <t>Win Prefetch Object</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Win Process Object </t>
+  </si>
+  <si>
+    <t>Win Registry Key Object</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Win Semaphore Object </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Win Service Object </t>
+  </si>
+  <si>
+    <t>Win System Object</t>
+  </si>
+  <si>
+    <t>Win System Restore Object</t>
+  </si>
+  <si>
+    <t>Win Task Object</t>
+  </si>
+  <si>
+    <t>Win Thread Object</t>
+  </si>
+  <si>
+    <t>Win User Account Object</t>
+  </si>
+  <si>
+    <t>Win Volume Object</t>
+  </si>
+  <si>
+    <t>Win Waitable Timer Object</t>
+  </si>
+  <si>
+    <t>X509 Certificate Object</t>
+  </si>
+  <si>
+    <t>Alternative_ID</t>
+  </si>
+  <si>
+    <t>Valid_Time_Position</t>
+  </si>
+  <si>
+    <t>indicator:ValidTimeType</t>
+  </si>
+  <si>
+    <t>cybox:ObservableType</t>
+  </si>
+  <si>
+    <t>Composite_Indicator_Expression</t>
+  </si>
+  <si>
+    <t>indicator:CompositeIndicatorExpressionType</t>
+  </si>
+  <si>
+    <t>Indicated_TTP</t>
+  </si>
+  <si>
+    <t>stixCommon:RelatedTTPType</t>
+  </si>
+  <si>
+    <t>Kill_Chain_Phases</t>
+  </si>
+  <si>
+    <t>stixCommon:KillChainPhasesReferenceType</t>
+  </si>
+  <si>
+    <t>Test_Mechanisms</t>
+  </si>
+  <si>
+    <t>indicator:TestMechanismsType</t>
+  </si>
+  <si>
+    <t>Likely_Impact</t>
+  </si>
+  <si>
+    <t>stixCommon:StatementType</t>
+  </si>
+  <si>
+    <t>Suggested_COAs</t>
+  </si>
+  <si>
+    <t>indicator:SuggestedCOAsType</t>
+  </si>
+  <si>
+    <t>Confidence</t>
+  </si>
+  <si>
+    <t>stixCommon:ConfidenceType</t>
+  </si>
+  <si>
+    <t>Sightings</t>
+  </si>
+  <si>
+    <t>indicator:SightingsType</t>
+  </si>
+  <si>
+    <t>Related_Indicators</t>
+  </si>
+  <si>
+    <t>indicator:RelatedIndicatorsType</t>
+  </si>
+  <si>
+    <t>Producer</t>
+  </si>
+  <si>
+    <t>indicator:IndicatorVersionType</t>
+  </si>
+  <si>
+    <t>@negate</t>
+  </si>
+  <si>
+    <t>xs:boolean</t>
+  </si>
+  <si>
+    <t>IndicatorType</t>
+  </si>
+  <si>
+    <t>CybOX Object</t>
+  </si>
+  <si>
+    <t>Properties</t>
+  </si>
+  <si>
+    <t>cybox:ObjectTypePropertiesType</t>
+  </si>
+  <si>
+    <t>FileObj:FileObjectType, AddressObject:AddressObjectType, EmailMessageObj:EmailMessageObjectType</t>
+  </si>
+  <si>
+    <t>http://cybox.mitre.org/cybox-2</t>
+  </si>
+  <si>
+    <t>cybox:Object</t>
+  </si>
+  <si>
+    <t>cybox</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -407,6 +768,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color rgb="FF1F497D"/>
@@ -447,6 +829,13 @@
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
@@ -501,7 +890,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -630,13 +1019,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDDDDDD"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFDDDDDD"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -667,26 +1070,44 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="28" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="29" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="20" fillId="0" borderId="13" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="2"/>
+    <xf numFmtId="0" fontId="31" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="14" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="14" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="6">
+    <cellStyle name="Bad" xfId="4" builtinId="27"/>
+    <cellStyle name="Good" xfId="3" builtinId="26"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="5" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -986,31 +1407,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.109375" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="67.6640625" customWidth="1"/>
-    <col min="2" max="2" width="34.5546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.5546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.6640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.5546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.109375" style="21" customWidth="1"/>
+    <col min="4" max="4" width="43.6640625" style="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="22" t="s">
         <v>59</v>
       </c>
       <c r="E1" s="15"/>
@@ -1020,135 +1441,135 @@
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" s="23" t="s">
+      <c r="B2" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="24" t="s">
         <v>60</v>
       </c>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
     </row>
-    <row r="3" spans="1:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" s="24" t="s">
+      <c r="B3" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" s="25" t="s">
         <v>61</v>
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" s="25" t="s">
+      <c r="B4" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" s="26" t="s">
         <v>62</v>
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
     </row>
-    <row r="5" spans="1:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" s="22" t="s">
+      <c r="B5" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="D5" s="23" t="s">
         <v>52</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
     </row>
-    <row r="6" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="D6" s="23" t="s">
+      <c r="B6" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" s="24" t="s">
         <v>63</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
     </row>
-    <row r="7" spans="1:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="C7" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="D7" s="26" t="s">
+      <c r="B7" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7" s="27" t="s">
         <v>64</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
     </row>
-    <row r="8" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
-      <c r="B8" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="D8" s="24" t="s">
+      <c r="B8" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="D8" s="25" t="s">
         <v>65</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
     </row>
-    <row r="9" spans="1:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="10"/>
-      <c r="B9" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="D9" s="27" t="s">
+      <c r="B9" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="D9" s="28" t="s">
         <v>66</v>
       </c>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
     </row>
-    <row r="10" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="15"/>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10" s="25" t="s">
+      <c r="C10" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" s="26" t="s">
         <v>62</v>
       </c>
       <c r="E10" s="15"/>
@@ -1156,13 +1577,13 @@
     </row>
     <row r="11" spans="1:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A11" s="15"/>
-      <c r="B11" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="C11" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" s="22" t="s">
+      <c r="B11" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>104</v>
+      </c>
+      <c r="D11" s="23" t="s">
         <v>52</v>
       </c>
       <c r="E11" s="15"/>
@@ -1170,48 +1591,394 @@
     </row>
     <row r="12" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15"/>
+      <c r="B12" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>105</v>
+      </c>
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
     </row>
-    <row r="13" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A13" s="15"/>
+      <c r="B13" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>106</v>
+      </c>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
     </row>
-    <row r="14" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15"/>
+      <c r="B14" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>107</v>
+      </c>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
     </row>
-    <row r="15" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A15" s="15"/>
+      <c r="B15" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>108</v>
+      </c>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
     </row>
-    <row r="16" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A16" s="15"/>
+      <c r="B16" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="33" t="s">
+        <v>109</v>
+      </c>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
     </row>
-    <row r="17" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A17" s="15"/>
+      <c r="B17" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="33" t="s">
+        <v>110</v>
+      </c>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
     </row>
-    <row r="18" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A18" s="15"/>
+      <c r="B18" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="33" t="s">
+        <v>111</v>
+      </c>
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
     </row>
-    <row r="19" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A19" s="15"/>
+      <c r="B19" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="26" t="s">
+        <v>112</v>
+      </c>
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
     </row>
-    <row r="20" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A20" s="15"/>
+      <c r="C20" s="33" t="s">
+        <v>113</v>
+      </c>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
+    </row>
+    <row r="21" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="26" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C22" s="33" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="33" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="26" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="26" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="26" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="26" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="33" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="33" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C30" s="33" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C31" s="33" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C32" s="33" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C33" s="33" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C34" s="26" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C35" s="33" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C36" s="33" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="37" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C37" s="33" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="38" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C38" s="26" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="39" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C39" s="26" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="40" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C40" s="26" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="41" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C41" s="33" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="42" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C42" s="33" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="43" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C43" s="33" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="44" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C44" s="33" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="45" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C45" s="33" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="46" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C46" s="33" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="47" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C47" s="33" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="48" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C48" s="33" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C49" s="33" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="50" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C50" s="33" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="51" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C51" s="33" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="52" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C52" s="33" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="53" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C53" s="33" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="54" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C54" s="33" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="55" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C55" s="33" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="56" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C56" s="33" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="57" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C57" s="33" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="58" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C58" s="33" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="59" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C59" s="33" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="60" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C60" s="33" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="61" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C61" s="33" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="62" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C62" s="33" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="63" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C63" s="33" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="64" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C64" s="33" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="65" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C65" s="33" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="66" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C66" s="33" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="67" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C67" s="33" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="68" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C68" s="33" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="69" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C69" s="26" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="70" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C70" s="33" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="71" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C71" s="33" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="72" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C72" s="33" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="73" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C73" s="33" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="74" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C74" s="33" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="75" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C75" s="33" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="76" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C76" s="33" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="77" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C77" s="33" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="78" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C78" s="33" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="79" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C79" s="33" t="s">
+        <v>172</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1222,8 +1989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.109375" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1243,7 +2010,7 @@
       <c r="B1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="32" t="s">
         <v>69</v>
       </c>
       <c r="D1" s="8" t="s">
@@ -1259,19 +2026,19 @@
         <v>11</v>
       </c>
       <c r="B2" s="17"/>
-      <c r="C2" s="20"/>
+      <c r="C2" s="21"/>
       <c r="D2" s="17"/>
       <c r="E2" s="17"/>
       <c r="F2" s="15"/>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="27" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="21" t="s">
         <v>71</v>
       </c>
       <c r="D3" s="15"/>
@@ -1285,7 +2052,7 @@
       <c r="B4" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="21" t="s">
         <v>72</v>
       </c>
       <c r="D4" s="15"/>
@@ -1293,13 +2060,13 @@
       <c r="F4" s="15"/>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="21" t="s">
         <v>73</v>
       </c>
       <c r="D5" s="15"/>
@@ -1307,13 +2074,13 @@
       <c r="F5" s="15"/>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="21" t="s">
         <v>74</v>
       </c>
       <c r="D6" s="15"/>
@@ -1327,7 +2094,7 @@
       <c r="B7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="21" t="s">
         <v>75</v>
       </c>
       <c r="D7" s="15"/>
@@ -1341,7 +2108,7 @@
       <c r="B8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="21" t="s">
         <v>76</v>
       </c>
       <c r="D8" s="15"/>
@@ -1355,7 +2122,7 @@
       <c r="B9" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="21" t="s">
         <v>77</v>
       </c>
       <c r="D9" s="15"/>
@@ -1369,7 +2136,7 @@
       <c r="B10" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="21" t="s">
         <v>78</v>
       </c>
       <c r="D10" s="15"/>
@@ -1383,7 +2150,7 @@
       <c r="B11" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="21" t="s">
         <v>79</v>
       </c>
       <c r="D11" s="15"/>
@@ -1391,13 +2158,13 @@
       <c r="F11" s="15"/>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="27" t="s">
         <v>24</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="21" t="s">
         <v>80</v>
       </c>
       <c r="D12" s="15"/>
@@ -1411,7 +2178,7 @@
       <c r="B13" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="21" t="s">
         <v>80</v>
       </c>
       <c r="D13" s="15"/>
@@ -1419,13 +2186,13 @@
       <c r="F13" s="15"/>
     </row>
     <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="26" t="s">
+      <c r="A14" s="27" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="21" t="s">
         <v>81</v>
       </c>
       <c r="D14" s="15"/>
@@ -1435,7 +2202,7 @@
       <c r="F14" s="15"/>
     </row>
     <row r="15" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="30" t="s">
         <v>68</v>
       </c>
       <c r="B15" s="15"/>
@@ -1445,13 +2212,15 @@
       <c r="F15" s="15"/>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="18"/>
+      <c r="C16" s="19" t="s">
+        <v>87</v>
+      </c>
       <c r="D16" s="15"/>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
@@ -1498,7 +2267,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.109375" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1518,7 +2287,7 @@
       <c r="B1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="32" t="s">
         <v>69</v>
       </c>
       <c r="D1" s="8" t="s">
@@ -1540,13 +2309,13 @@
       <c r="F2" s="15"/>
     </row>
     <row r="3" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="27" t="s">
         <v>29</v>
       </c>
       <c r="B3" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="21" t="s">
         <v>82</v>
       </c>
       <c r="D3" s="15"/>
@@ -1554,13 +2323,13 @@
       <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="27" t="s">
         <v>30</v>
       </c>
       <c r="B4" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="21" t="s">
         <v>83</v>
       </c>
       <c r="D4" s="11" t="s">
@@ -1578,7 +2347,7 @@
       <c r="B5" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="21" t="s">
         <v>84</v>
       </c>
       <c r="D5" s="15"/>
@@ -1586,13 +2355,13 @@
       <c r="F5" s="15"/>
     </row>
     <row r="6" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="27" t="s">
         <v>34</v>
       </c>
       <c r="B6" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="21" t="s">
         <v>85</v>
       </c>
       <c r="D6" s="15"/>
@@ -1600,13 +2369,13 @@
       <c r="F6" s="15"/>
     </row>
     <row r="7" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="27" t="s">
         <v>35</v>
       </c>
       <c r="B7" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="21" t="s">
         <v>86</v>
       </c>
       <c r="D7" s="15"/>
@@ -1616,7 +2385,7 @@
     <row r="8" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="15"/>
       <c r="B8" s="15"/>
-      <c r="C8" s="30"/>
+      <c r="C8" s="31"/>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
@@ -1680,7 +2449,7 @@
     <row r="16" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="15"/>
       <c r="B16" s="15"/>
-      <c r="C16" s="18"/>
+      <c r="C16" s="19"/>
       <c r="D16" s="15"/>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
@@ -1727,7 +2496,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.109375" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1747,7 +2516,7 @@
       <c r="B1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="29" t="s">
         <v>69</v>
       </c>
       <c r="D1" s="8" t="s">
@@ -1768,14 +2537,14 @@
       <c r="E2" s="17"/>
       <c r="F2" s="15"/>
     </row>
-    <row r="3" spans="1:6" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
+    <row r="3" spans="1:6" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="21" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1786,17 +2555,272 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="55.109375" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.44140625" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="13" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="15"/>
+    </row>
+    <row r="2" spans="1:6" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="35" t="s">
+        <v>199</v>
+      </c>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+    </row>
+    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A4" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="36" t="s">
+        <v>173</v>
+      </c>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A9" s="36" t="s">
+        <v>174</v>
+      </c>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="36" t="s">
+        <v>177</v>
+      </c>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="36" t="s">
+        <v>179</v>
+      </c>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="37" t="s">
+        <v>183</v>
+      </c>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="36" t="s">
+        <v>185</v>
+      </c>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="36" t="s">
+        <v>187</v>
+      </c>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="36" t="s">
+        <v>189</v>
+      </c>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="36" t="s">
+        <v>191</v>
+      </c>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="36" t="s">
+        <v>193</v>
+      </c>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="37" t="s">
+        <v>195</v>
+      </c>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="36" t="s">
+        <v>197</v>
+      </c>
+      <c r="B23" s="21"/>
+      <c r="C23" s="21" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A24" s="35" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="27" x14ac:dyDescent="0.3">
+      <c r="A25" s="27" t="s">
+        <v>201</v>
+      </c>
+      <c r="B25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" t="s">
+        <v>202</v>
+      </c>
+      <c r="D25" t="s">
+        <v>203</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.88671875" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.88671875" customWidth="1"/>
     <col min="2" max="2" width="27.88671875" customWidth="1"/>
-    <col min="3" max="4" width="9.88671875" style="20"/>
+    <col min="3" max="4" width="9.88671875" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="13" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -1806,8 +2830,8 @@
       <c r="B1" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
       <c r="E1" s="15"/>
     </row>
     <row r="2" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -1855,7 +2879,7 @@
       <c r="F5" s="15"/>
     </row>
     <row r="6" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="20" t="s">
         <v>43</v>
       </c>
       <c r="B6" s="15" t="s">
@@ -1865,7 +2889,7 @@
       <c r="F6" s="15"/>
     </row>
     <row r="7" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="20" t="s">
         <v>45</v>
       </c>
       <c r="B7" s="15" t="s">
@@ -1875,8 +2899,12 @@
       <c r="F7" s="15"/>
     </row>
     <row r="8" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
+      <c r="A8" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>206</v>
+      </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
     </row>
@@ -1956,35 +2984,36 @@
   <hyperlinks>
     <hyperlink ref="A6" r:id="rId1"/>
     <hyperlink ref="A7" r:id="rId2"/>
+    <hyperlink ref="A8" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.88671875" customWidth="1"/>
     <col min="2" max="2" width="100" customWidth="1"/>
-    <col min="3" max="4" width="17.109375" style="20"/>
+    <col min="3" max="4" width="17.109375" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="13" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
       <c r="E1" s="15"/>
     </row>
     <row r="2" spans="1:5" ht="12.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -2007,7 +3036,7 @@
       <c r="A4" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="21" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2017,6 +3046,14 @@
       </c>
       <c r="B5" t="s">
         <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>200</v>
+      </c>
+      <c r="B6" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added field types to Indicator sheet
</commit_message>
<xml_diff>
--- a/examples/Example_Profile.xlsx
+++ b/examples/Example_Profile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="516" yWindow="612" windowWidth="15996" windowHeight="5448" activeTab="5"/>
+    <workbookView xWindow="516" yWindow="612" windowWidth="15996" windowHeight="5448" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="207">
   <si>
     <t>Profile Information</t>
   </si>
@@ -2496,7 +2496,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.109375" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2557,8 +2557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2599,7 +2599,9 @@
       <c r="A3" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="21"/>
+      <c r="B3" s="21" t="s">
+        <v>13</v>
+      </c>
       <c r="C3" s="21" t="s">
         <v>80</v>
       </c>
@@ -2608,7 +2610,9 @@
       <c r="A4" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="21"/>
+      <c r="B4" s="21" t="s">
+        <v>15</v>
+      </c>
       <c r="C4" s="21" t="s">
         <v>80</v>
       </c>
@@ -2617,7 +2621,9 @@
       <c r="A5" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="21"/>
+      <c r="B5" s="21" t="s">
+        <v>13</v>
+      </c>
       <c r="C5" s="21" t="s">
         <v>82</v>
       </c>
@@ -2626,7 +2632,9 @@
       <c r="A6" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="B6" s="21"/>
+      <c r="B6" s="21" t="s">
+        <v>13</v>
+      </c>
       <c r="C6" s="21" t="s">
         <v>83</v>
       </c>
@@ -2635,7 +2643,9 @@
       <c r="A7" s="36" t="s">
         <v>173</v>
       </c>
-      <c r="B7" s="21"/>
+      <c r="B7" s="21" t="s">
+        <v>15</v>
+      </c>
       <c r="C7" s="21" t="s">
         <v>82</v>
       </c>
@@ -2644,7 +2654,9 @@
       <c r="A8" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="21"/>
+      <c r="B8" s="21" t="s">
+        <v>15</v>
+      </c>
       <c r="C8" s="21" t="s">
         <v>84</v>
       </c>
@@ -2653,7 +2665,9 @@
       <c r="A9" s="36" t="s">
         <v>174</v>
       </c>
-      <c r="B9" s="21"/>
+      <c r="B9" s="21" t="s">
+        <v>15</v>
+      </c>
       <c r="C9" s="21" t="s">
         <v>175</v>
       </c>
@@ -2662,7 +2676,9 @@
       <c r="A10" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="B10" s="21"/>
+      <c r="B10" s="21" t="s">
+        <v>13</v>
+      </c>
       <c r="C10" s="21" t="s">
         <v>176</v>
       </c>
@@ -2671,7 +2687,9 @@
       <c r="A11" s="36" t="s">
         <v>177</v>
       </c>
-      <c r="B11" s="21"/>
+      <c r="B11" s="21" t="s">
+        <v>15</v>
+      </c>
       <c r="C11" s="21" t="s">
         <v>178</v>
       </c>
@@ -2680,7 +2698,9 @@
       <c r="A12" s="36" t="s">
         <v>179</v>
       </c>
-      <c r="B12" s="21"/>
+      <c r="B12" s="21" t="s">
+        <v>15</v>
+      </c>
       <c r="C12" s="21" t="s">
         <v>180</v>
       </c>
@@ -2689,7 +2709,9 @@
       <c r="A13" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="B13" s="21"/>
+      <c r="B13" s="21" t="s">
+        <v>15</v>
+      </c>
       <c r="C13" s="21" t="s">
         <v>182</v>
       </c>
@@ -2698,7 +2720,9 @@
       <c r="A14" s="37" t="s">
         <v>183</v>
       </c>
-      <c r="B14" s="21"/>
+      <c r="B14" s="21" t="s">
+        <v>19</v>
+      </c>
       <c r="C14" s="21" t="s">
         <v>184</v>
       </c>
@@ -2707,7 +2731,9 @@
       <c r="A15" s="36" t="s">
         <v>185</v>
       </c>
-      <c r="B15" s="21"/>
+      <c r="B15" s="21" t="s">
+        <v>15</v>
+      </c>
       <c r="C15" s="21" t="s">
         <v>186</v>
       </c>
@@ -2716,7 +2742,9 @@
       <c r="A16" s="36" t="s">
         <v>187</v>
       </c>
-      <c r="B16" s="21"/>
+      <c r="B16" s="21" t="s">
+        <v>15</v>
+      </c>
       <c r="C16" s="21" t="s">
         <v>188</v>
       </c>
@@ -2725,7 +2753,9 @@
       <c r="A17" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="21"/>
+      <c r="B17" s="21" t="s">
+        <v>19</v>
+      </c>
       <c r="C17" s="21" t="s">
         <v>85</v>
       </c>
@@ -2734,7 +2764,9 @@
       <c r="A18" s="36" t="s">
         <v>189</v>
       </c>
-      <c r="B18" s="21"/>
+      <c r="B18" s="21" t="s">
+        <v>15</v>
+      </c>
       <c r="C18" s="21" t="s">
         <v>190</v>
       </c>
@@ -2743,7 +2775,9 @@
       <c r="A19" s="36" t="s">
         <v>191</v>
       </c>
-      <c r="B19" s="21"/>
+      <c r="B19" s="21" t="s">
+        <v>15</v>
+      </c>
       <c r="C19" s="21" t="s">
         <v>192</v>
       </c>
@@ -2752,7 +2786,9 @@
       <c r="A20" s="36" t="s">
         <v>193</v>
       </c>
-      <c r="B20" s="21"/>
+      <c r="B20" s="21" t="s">
+        <v>15</v>
+      </c>
       <c r="C20" s="21" t="s">
         <v>194</v>
       </c>
@@ -2761,7 +2797,9 @@
       <c r="A21" s="37" t="s">
         <v>195</v>
       </c>
-      <c r="B21" s="21"/>
+      <c r="B21" s="21" t="s">
+        <v>19</v>
+      </c>
       <c r="C21" s="21" t="s">
         <v>86</v>
       </c>
@@ -2770,7 +2808,9 @@
       <c r="A22" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="21"/>
+      <c r="B22" s="21" t="s">
+        <v>19</v>
+      </c>
       <c r="C22" s="21" t="s">
         <v>196</v>
       </c>
@@ -2779,7 +2819,9 @@
       <c r="A23" s="36" t="s">
         <v>197</v>
       </c>
-      <c r="B23" s="21"/>
+      <c r="B23" s="21" t="s">
+        <v>15</v>
+      </c>
       <c r="C23" s="21" t="s">
         <v>198</v>
       </c>
@@ -2812,7 +2854,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updates to example profile
</commit_message>
<xml_diff>
--- a/examples/Example_Profile.xlsx
+++ b/examples/Example_Profile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="516" yWindow="612" windowWidth="15996" windowHeight="5448" activeTab="4"/>
+    <workbookView xWindow="516" yWindow="612" windowWidth="15996" windowHeight="5448" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="209">
   <si>
     <t>Profile Information</t>
   </si>
@@ -115,9 +115,6 @@
     <t>Package_Intent</t>
   </si>
   <si>
-    <t>stixVocabs:PackageIntentVocab-1.0, stixVocabs:HighMediumLowVocab-1.0</t>
-  </si>
-  <si>
     <t>Indicators - Phishing</t>
   </si>
   <si>
@@ -641,6 +638,15 @@
   </si>
   <si>
     <t>cybox</t>
+  </si>
+  <si>
+    <t>PackageIntentVocab-1.0</t>
+  </si>
+  <si>
+    <t>HighMediumLowVocab-1.0</t>
+  </si>
+  <si>
+    <t>stixVocabs:PackageIntentVocab-1.0</t>
   </si>
 </sst>
 </file>
@@ -1039,7 +1045,7 @@
     <xf numFmtId="0" fontId="22" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1101,6 +1107,7 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="4" builtinId="27"/>
@@ -1410,7 +1417,7 @@
   <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.109375" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1426,13 +1433,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C1" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="22" t="s">
         <v>58</v>
-      </c>
-      <c r="D1" s="22" t="s">
-        <v>59</v>
       </c>
       <c r="E1" s="15"/>
       <c r="F1" s="15"/>
@@ -1442,13 +1449,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
@@ -1458,13 +1465,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
@@ -1474,13 +1481,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
@@ -1490,13 +1497,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
@@ -1506,13 +1513,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
@@ -1522,13 +1529,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
@@ -1536,13 +1543,13 @@
     <row r="8" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
       <c r="B8" s="33" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
@@ -1550,13 +1557,13 @@
     <row r="9" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="10"/>
       <c r="B9" s="33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
@@ -1564,13 +1571,13 @@
     <row r="10" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="15"/>
       <c r="B10" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
@@ -1578,13 +1585,13 @@
     <row r="11" spans="1:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A11" s="15"/>
       <c r="B11" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
@@ -1592,10 +1599,10 @@
     <row r="12" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15"/>
       <c r="B12" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C12" s="33" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
@@ -1603,10 +1610,10 @@
     <row r="13" spans="1:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A13" s="15"/>
       <c r="B13" s="22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
@@ -1614,10 +1621,10 @@
     <row r="14" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15"/>
       <c r="B14" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
@@ -1625,10 +1632,10 @@
     <row r="15" spans="1:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A15" s="15"/>
       <c r="B15" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
@@ -1636,10 +1643,10 @@
     <row r="16" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A16" s="15"/>
       <c r="B16" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C16" s="33" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
@@ -1647,337 +1654,343 @@
     <row r="17" spans="1:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A17" s="15"/>
       <c r="B17" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C17" s="33" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
     </row>
     <row r="18" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A18" s="15"/>
-      <c r="B18" s="23" t="s">
-        <v>52</v>
+      <c r="B18" s="18" t="s">
+        <v>206</v>
       </c>
       <c r="C18" s="33" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
     </row>
-    <row r="19" spans="1:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="15"/>
-      <c r="B19" s="22" t="s">
-        <v>57</v>
+      <c r="B19" s="18" t="s">
+        <v>207</v>
       </c>
       <c r="C19" s="26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
     </row>
-    <row r="20" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20" s="15"/>
+      <c r="B20" s="23" t="s">
+        <v>51</v>
+      </c>
       <c r="C20" s="33" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
     </row>
-    <row r="21" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B21" s="22" t="s">
+        <v>56</v>
+      </c>
       <c r="C21" s="26" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="14.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="C22" s="33" t="s">
         <v>114</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="33" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C23" s="33" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C24" s="26" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C25" s="26" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C26" s="26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C27" s="26" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C28" s="33" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C29" s="33" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C30" s="33" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C31" s="33" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C32" s="33" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="33" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C33" s="33" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="34" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C34" s="26" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="35" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C35" s="33" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="36" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C36" s="33" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="37" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C37" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="38" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C38" s="26" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="39" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C39" s="26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="40" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C40" s="26" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="41" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C41" s="33" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="42" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C42" s="33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="43" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C43" s="33" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="44" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C44" s="33" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="45" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C45" s="33" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="46" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C46" s="33" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="47" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C47" s="33" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="48" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C48" s="33" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="49" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C49" s="33" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="50" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C50" s="33" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="51" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C51" s="33" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="52" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C52" s="33" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="53" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C53" s="33" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="54" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C54" s="33" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="55" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C55" s="33" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="56" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C56" s="33" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="57" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C57" s="33" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="58" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C58" s="33" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="59" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C59" s="33" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="60" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C60" s="33" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="61" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C61" s="33" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="62" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C62" s="33" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="63" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C63" s="33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="64" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C64" s="33" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="65" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C65" s="33" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="66" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C66" s="33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="67" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C67" s="33" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="68" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C68" s="33" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="69" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C69" s="26" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="70" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C70" s="33" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="71" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C71" s="33" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="72" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C72" s="33" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="73" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C73" s="33" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="74" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C74" s="33" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="75" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C75" s="33" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="76" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C76" s="33" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="77" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C77" s="33" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="78" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C78" s="33" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="79" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C79" s="33" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -2011,7 +2024,7 @@
         <v>8</v>
       </c>
       <c r="C1" s="32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>9</v>
@@ -2039,7 +2052,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
@@ -2053,7 +2066,7 @@
         <v>15</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
@@ -2067,7 +2080,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
@@ -2081,7 +2094,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
@@ -2095,7 +2108,7 @@
         <v>19</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
@@ -2109,7 +2122,7 @@
         <v>19</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
@@ -2123,7 +2136,7 @@
         <v>15</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
@@ -2137,7 +2150,7 @@
         <v>19</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
@@ -2151,7 +2164,7 @@
         <v>19</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
@@ -2165,7 +2178,7 @@
         <v>13</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
@@ -2179,7 +2192,7 @@
         <v>15</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
@@ -2193,7 +2206,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="11" t="s">
@@ -2203,7 +2216,7 @@
     </row>
     <row r="15" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A15" s="30" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
@@ -2213,13 +2226,13 @@
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16" s="19" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D16" s="15"/>
       <c r="E16" s="15"/>
@@ -2266,8 +2279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.109375" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2288,7 +2301,7 @@
         <v>8</v>
       </c>
       <c r="C1" s="32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>9</v>
@@ -2316,7 +2329,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
@@ -2330,25 +2343,25 @@
         <v>13</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="D4" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="39" t="s">
+        <v>208</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>31</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>32</v>
       </c>
       <c r="F4" s="15"/>
     </row>
     <row r="5" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" s="15" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
@@ -2356,13 +2369,13 @@
     </row>
     <row r="6" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
@@ -2370,13 +2383,13 @@
     </row>
     <row r="7" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
@@ -2517,7 +2530,7 @@
         <v>8</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>9</v>
@@ -2529,7 +2542,7 @@
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
@@ -2545,7 +2558,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -2557,7 +2570,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -2578,7 +2591,7 @@
         <v>8</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>9</v>
@@ -2590,7 +2603,7 @@
     </row>
     <row r="2" spans="1:6" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B2" s="21"/>
       <c r="C2" s="21"/>
@@ -2603,7 +2616,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
@@ -2614,7 +2627,7 @@
         <v>15</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
@@ -2625,183 +2638,183 @@
         <v>13</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B6" s="21" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="36" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B7" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="36" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A9" s="36" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B9" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B10" s="21" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="36" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B11" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="36" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B12" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="36" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B13" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="37" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B14" s="21" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="36" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B15" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="36" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B16" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B17" s="21" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="36" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B18" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="36" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B19" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="36" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B20" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="37" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B21" s="21" t="s">
         <v>19</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -2812,37 +2825,37 @@
         <v>19</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="36" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B23" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A24" s="35" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="27" x14ac:dyDescent="0.3">
       <c r="A25" s="27" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B25" t="s">
         <v>13</v>
       </c>
       <c r="C25" t="s">
+        <v>201</v>
+      </c>
+      <c r="D25" t="s">
         <v>202</v>
-      </c>
-      <c r="D25" t="s">
-        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -2867,10 +2880,10 @@
   <sheetData>
     <row r="1" spans="1:6" s="13" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>37</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>38</v>
       </c>
       <c r="C1" s="21"/>
       <c r="D1" s="21"/>
@@ -2882,7 +2895,7 @@
         <v>http://www.w3.org/2001/XMLSchema-instance</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
@@ -2893,7 +2906,7 @@
         <v>http://stix.mitre.org/stix-1</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
@@ -2904,7 +2917,7 @@
         <v>http://stix.mitre.org/common-1</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
@@ -2915,37 +2928,37 @@
         <v>http://stix.mitre.org/default_vocabularies-1</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
     </row>
     <row r="6" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="15" t="s">
         <v>43</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>44</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
     </row>
     <row r="7" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="15" t="s">
         <v>45</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>46</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
     </row>
     <row r="8" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
@@ -3049,10 +3062,10 @@
   <sheetData>
     <row r="1" spans="1:5" s="13" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C1" s="21"/>
       <c r="D1" s="21"/>
@@ -3063,7 +3076,7 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3071,31 +3084,31 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated @version allowed values in profile
</commit_message>
<xml_diff>
--- a/examples/Example_Profile.xlsx
+++ b/examples/Example_Profile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="516" yWindow="612" windowWidth="15996" windowHeight="5448" activeTab="2"/>
+    <workbookView xWindow="516" yWindow="612" windowWidth="15996" windowHeight="5448" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -103,9 +103,6 @@
     <t>@version</t>
   </si>
   <si>
-    <t>1.0, 1.0.1</t>
-  </si>
-  <si>
     <t>STIXHeaderType</t>
   </si>
   <si>
@@ -625,9 +622,6 @@
     <t>Properties</t>
   </si>
   <si>
-    <t>cybox:ObjectTypePropertiesType</t>
-  </si>
-  <si>
     <t>FileObj:FileObjectType, AddressObject:AddressObjectType, EmailMessageObj:EmailMessageObjectType</t>
   </si>
   <si>
@@ -647,6 +641,12 @@
   </si>
   <si>
     <t>stixVocabs:PackageIntentVocab-1.0</t>
+  </si>
+  <si>
+    <t>cybox:ObjectPropertiesType</t>
+  </si>
+  <si>
+    <t>1.0.1, 1.1</t>
   </si>
 </sst>
 </file>
@@ -1433,13 +1433,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C1" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="22" t="s">
         <v>57</v>
-      </c>
-      <c r="D1" s="22" t="s">
-        <v>58</v>
       </c>
       <c r="E1" s="15"/>
       <c r="F1" s="15"/>
@@ -1449,13 +1449,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
@@ -1465,13 +1465,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
@@ -1481,13 +1481,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
@@ -1497,13 +1497,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
@@ -1513,13 +1513,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
@@ -1529,13 +1529,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
@@ -1543,13 +1543,13 @@
     <row r="8" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
       <c r="B8" s="33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
@@ -1557,13 +1557,13 @@
     <row r="9" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="10"/>
       <c r="B9" s="33" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
@@ -1571,13 +1571,13 @@
     <row r="10" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="15"/>
       <c r="B10" s="23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
@@ -1585,13 +1585,13 @@
     <row r="11" spans="1:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A11" s="15"/>
       <c r="B11" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
@@ -1599,10 +1599,10 @@
     <row r="12" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15"/>
       <c r="B12" s="23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" s="33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
@@ -1610,10 +1610,10 @@
     <row r="13" spans="1:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A13" s="15"/>
       <c r="B13" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
@@ -1621,10 +1621,10 @@
     <row r="14" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15"/>
       <c r="B14" s="23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
@@ -1632,10 +1632,10 @@
     <row r="15" spans="1:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A15" s="15"/>
       <c r="B15" s="22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
@@ -1643,10 +1643,10 @@
     <row r="16" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A16" s="15"/>
       <c r="B16" s="23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C16" s="33" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
@@ -1654,10 +1654,10 @@
     <row r="17" spans="1:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A17" s="15"/>
       <c r="B17" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C17" s="33" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
@@ -1665,10 +1665,10 @@
     <row r="18" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A18" s="15"/>
       <c r="B18" s="18" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C18" s="33" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
@@ -1676,10 +1676,10 @@
     <row r="19" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="15"/>
       <c r="B19" s="18" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C19" s="26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
@@ -1687,310 +1687,310 @@
     <row r="20" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20" s="15"/>
       <c r="B20" s="23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C20" s="33" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
     </row>
     <row r="21" spans="1:6" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B21" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C21" s="26" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="14.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C22" s="33" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C23" s="33" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C24" s="26" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C25" s="26" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C26" s="26" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C27" s="26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C28" s="33" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C29" s="33" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C30" s="33" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C31" s="33" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C32" s="33" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="33" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C33" s="33" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="34" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C34" s="26" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="35" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C35" s="33" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="36" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C36" s="33" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="37" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C37" s="33" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="38" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C38" s="26" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="39" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C39" s="26" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="40" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C40" s="26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="41" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C41" s="33" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="42" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C42" s="33" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="43" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C43" s="33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="44" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C44" s="33" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="45" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C45" s="33" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="46" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C46" s="33" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="47" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C47" s="33" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="48" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C48" s="33" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="49" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C49" s="33" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="50" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C50" s="33" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="51" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C51" s="33" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="52" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C52" s="33" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="53" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C53" s="33" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="54" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C54" s="33" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="55" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C55" s="33" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="56" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C56" s="33" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="57" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C57" s="33" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="58" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C58" s="33" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="59" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C59" s="33" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="60" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C60" s="33" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="61" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C61" s="33" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="62" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C62" s="33" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="63" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C63" s="33" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="64" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C64" s="33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="65" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C65" s="33" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="66" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C66" s="33" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="67" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C67" s="33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="68" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C68" s="33" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="69" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C69" s="26" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="70" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C70" s="33" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="71" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C71" s="33" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="72" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C72" s="33" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="73" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C73" s="33" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="74" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C74" s="33" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="75" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C75" s="33" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="76" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C76" s="33" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="77" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C77" s="33" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="78" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C78" s="33" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="79" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C79" s="33" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -2002,8 +2002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.109375" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2024,7 +2024,7 @@
         <v>8</v>
       </c>
       <c r="C1" s="32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>9</v>
@@ -2052,7 +2052,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
@@ -2066,7 +2066,7 @@
         <v>15</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
@@ -2080,7 +2080,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
@@ -2094,7 +2094,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
@@ -2108,7 +2108,7 @@
         <v>19</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
@@ -2122,7 +2122,7 @@
         <v>19</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
@@ -2136,7 +2136,7 @@
         <v>15</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
@@ -2150,7 +2150,7 @@
         <v>19</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
@@ -2164,7 +2164,7 @@
         <v>19</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
@@ -2178,7 +2178,7 @@
         <v>13</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
@@ -2192,7 +2192,7 @@
         <v>15</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
@@ -2206,17 +2206,17 @@
         <v>13</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D14" s="15"/>
-      <c r="E14" s="11" t="s">
-        <v>27</v>
+      <c r="E14" s="39" t="s">
+        <v>208</v>
       </c>
       <c r="F14" s="15"/>
     </row>
     <row r="15" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A15" s="30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
@@ -2226,13 +2226,13 @@
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B16" s="19" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D16" s="15"/>
       <c r="E16" s="15"/>
@@ -2279,7 +2279,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -2301,7 +2301,7 @@
         <v>8</v>
       </c>
       <c r="C1" s="32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>9</v>
@@ -2313,7 +2313,7 @@
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
@@ -2323,13 +2323,13 @@
     </row>
     <row r="3" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
@@ -2337,31 +2337,31 @@
     </row>
     <row r="4" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D4" s="39" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F4" s="15"/>
     </row>
     <row r="5" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="15" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
@@ -2369,13 +2369,13 @@
     </row>
     <row r="6" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
@@ -2383,13 +2383,13 @@
     </row>
     <row r="7" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
@@ -2508,8 +2508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.109375" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2530,7 +2530,7 @@
         <v>8</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>9</v>
@@ -2542,7 +2542,7 @@
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
@@ -2552,13 +2552,13 @@
     </row>
     <row r="3" spans="1:6" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" s="21" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -2570,8 +2570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2591,7 +2591,7 @@
         <v>8</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>9</v>
@@ -2603,7 +2603,7 @@
     </row>
     <row r="2" spans="1:6" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B2" s="21"/>
       <c r="C2" s="21"/>
@@ -2616,7 +2616,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
@@ -2627,194 +2627,194 @@
         <v>15</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="21" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B6" s="21" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="36" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B7" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A9" s="36" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B9" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B10" s="21" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B11" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="36" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B12" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="36" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B13" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="37" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B14" s="21" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="36" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B15" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="36" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B16" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="37" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17" s="21" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="36" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B18" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="36" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B19" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="36" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B20" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="37" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B21" s="21" t="s">
         <v>19</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -2825,37 +2825,37 @@
         <v>19</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="36" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B23" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A24" s="35" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="27" x14ac:dyDescent="0.3">
       <c r="A25" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B25" t="s">
         <v>13</v>
       </c>
       <c r="C25" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="D25" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -2868,7 +2868,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.88671875" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2880,10 +2880,10 @@
   <sheetData>
     <row r="1" spans="1:6" s="13" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>36</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>37</v>
       </c>
       <c r="C1" s="21"/>
       <c r="D1" s="21"/>
@@ -2895,7 +2895,7 @@
         <v>http://www.w3.org/2001/XMLSchema-instance</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
@@ -2906,7 +2906,7 @@
         <v>http://stix.mitre.org/stix-1</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
@@ -2917,7 +2917,7 @@
         <v>http://stix.mitre.org/common-1</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
@@ -2928,37 +2928,37 @@
         <v>http://stix.mitre.org/default_vocabularies-1</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
     </row>
     <row r="6" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="15" t="s">
         <v>42</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>43</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
     </row>
     <row r="7" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="15" t="s">
         <v>44</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>45</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
     </row>
     <row r="8" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="B8" s="19" t="s">
         <v>203</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>205</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
@@ -3050,7 +3050,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3062,10 +3062,10 @@
   <sheetData>
     <row r="1" spans="1:5" s="13" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C1" s="21"/>
       <c r="D1" s="21"/>
@@ -3076,39 +3076,39 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B6" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed bug where schematron tests declared incorrect namespace for fields. This required a new 'Type Namespace' column in the profile. Fixed issue where duplicate errors were being reported
</commit_message>
<xml_diff>
--- a/examples/Example_Profile.xlsx
+++ b/examples/Example_Profile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="516" yWindow="612" windowWidth="15996" windowHeight="5448" activeTab="1"/>
+    <workbookView xWindow="516" yWindow="612" windowWidth="15996" windowHeight="5448" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="214">
   <si>
     <t>Profile Information</t>
   </si>
@@ -157,9 +157,6 @@
     <t>incident</t>
   </si>
   <si>
-    <t>Label</t>
-  </si>
-  <si>
     <t>stix:STIX_Package, stix:Package</t>
   </si>
   <si>
@@ -647,6 +644,24 @@
   </si>
   <si>
     <t>1.0.1, 1.1</t>
+  </si>
+  <si>
+    <t>stix:Indicator</t>
+  </si>
+  <si>
+    <t>Type Namespace</t>
+  </si>
+  <si>
+    <t>http://stix.mitre.org/stix-1</t>
+  </si>
+  <si>
+    <t>http://stix.mitre.org/Indicator-2</t>
+  </si>
+  <si>
+    <t>indicator</t>
+  </si>
+  <si>
+    <t>Type Label</t>
   </si>
 </sst>
 </file>
@@ -1433,13 +1448,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C1" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="22" t="s">
         <v>56</v>
-      </c>
-      <c r="D1" s="22" t="s">
-        <v>57</v>
       </c>
       <c r="E1" s="15"/>
       <c r="F1" s="15"/>
@@ -1449,13 +1464,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
@@ -1465,13 +1480,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
@@ -1484,10 +1499,10 @@
         <v>34</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
@@ -1497,13 +1512,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
@@ -1513,13 +1528,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
@@ -1529,13 +1544,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
@@ -1543,13 +1558,13 @@
     <row r="8" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
       <c r="B8" s="33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
@@ -1557,13 +1572,13 @@
     <row r="9" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="10"/>
       <c r="B9" s="33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
@@ -1571,13 +1586,13 @@
     <row r="10" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="15"/>
       <c r="B10" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
@@ -1585,13 +1600,13 @@
     <row r="11" spans="1:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A11" s="15"/>
       <c r="B11" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
@@ -1599,10 +1614,10 @@
     <row r="12" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15"/>
       <c r="B12" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C12" s="33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
@@ -1610,10 +1625,10 @@
     <row r="13" spans="1:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A13" s="15"/>
       <c r="B13" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
@@ -1621,10 +1636,10 @@
     <row r="14" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15"/>
       <c r="B14" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
@@ -1632,10 +1647,10 @@
     <row r="15" spans="1:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A15" s="15"/>
       <c r="B15" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
@@ -1643,10 +1658,10 @@
     <row r="16" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A16" s="15"/>
       <c r="B16" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C16" s="33" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
@@ -1654,10 +1669,10 @@
     <row r="17" spans="1:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A17" s="15"/>
       <c r="B17" s="22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C17" s="33" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
@@ -1665,10 +1680,10 @@
     <row r="18" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A18" s="15"/>
       <c r="B18" s="18" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C18" s="33" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
@@ -1676,10 +1691,10 @@
     <row r="19" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="15"/>
       <c r="B19" s="18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C19" s="26" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
@@ -1687,310 +1702,310 @@
     <row r="20" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20" s="15"/>
       <c r="B20" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C20" s="33" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
     </row>
     <row r="21" spans="1:6" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B21" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C21" s="26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="14.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C22" s="33" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C23" s="33" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C24" s="26" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C25" s="26" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C26" s="26" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C27" s="26" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C28" s="33" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C29" s="33" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C30" s="33" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C31" s="33" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C32" s="33" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="33" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C33" s="33" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C34" s="26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="35" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C35" s="33" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="36" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C36" s="33" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="37" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C37" s="33" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C38" s="26" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="39" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C39" s="26" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="40" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C40" s="26" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="41" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C41" s="33" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="42" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C42" s="33" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="43" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C43" s="33" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="44" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C44" s="33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="45" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C45" s="33" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="46" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C46" s="33" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="47" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C47" s="33" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="48" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C48" s="33" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="49" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C49" s="33" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="50" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C50" s="33" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="51" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C51" s="33" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="52" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C52" s="33" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="53" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C53" s="33" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="54" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C54" s="33" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="55" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C55" s="33" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="56" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C56" s="33" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="57" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C57" s="33" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="58" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C58" s="33" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="59" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C59" s="33" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="60" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C60" s="33" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="61" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C61" s="33" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="62" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C62" s="33" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="63" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C63" s="33" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="64" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C64" s="33" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="65" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C65" s="33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="66" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C66" s="33" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="67" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C67" s="33" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="68" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C68" s="33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="69" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C69" s="26" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="70" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C70" s="33" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="71" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C71" s="33" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="72" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C72" s="33" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="73" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C73" s="33" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="74" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C74" s="33" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="75" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C75" s="33" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="76" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C76" s="33" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="77" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C77" s="33" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="78" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C78" s="33" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="79" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C79" s="33" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -2002,8 +2017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.109375" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2024,7 +2039,7 @@
         <v>8</v>
       </c>
       <c r="C1" s="32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>9</v>
@@ -2052,7 +2067,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
@@ -2066,7 +2081,7 @@
         <v>15</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
@@ -2080,7 +2095,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
@@ -2094,7 +2109,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
@@ -2108,7 +2123,7 @@
         <v>19</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
@@ -2122,7 +2137,7 @@
         <v>19</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
@@ -2136,7 +2151,7 @@
         <v>15</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
@@ -2150,7 +2165,7 @@
         <v>19</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
@@ -2164,7 +2179,7 @@
         <v>19</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
@@ -2178,7 +2193,7 @@
         <v>13</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
@@ -2192,7 +2207,7 @@
         <v>15</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
@@ -2206,17 +2221,17 @@
         <v>13</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="39" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F14" s="15"/>
     </row>
     <row r="15" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A15" s="30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
@@ -2232,7 +2247,7 @@
         <v>13</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D16" s="15"/>
       <c r="E16" s="15"/>
@@ -2301,7 +2316,7 @@
         <v>8</v>
       </c>
       <c r="C1" s="32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>9</v>
@@ -2329,7 +2344,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
@@ -2343,10 +2358,10 @@
         <v>13</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D4" s="39" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>30</v>
@@ -2361,7 +2376,7 @@
         <v>15</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
@@ -2375,7 +2390,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
@@ -2389,7 +2404,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
@@ -2530,7 +2545,7 @@
         <v>8</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>9</v>
@@ -2558,7 +2573,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -2571,7 +2586,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2591,7 +2606,7 @@
         <v>8</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>9</v>
@@ -2603,7 +2618,7 @@
     </row>
     <row r="2" spans="1:6" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B2" s="21"/>
       <c r="C2" s="21"/>
@@ -2616,7 +2631,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
@@ -2627,7 +2642,7 @@
         <v>15</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
@@ -2638,29 +2653,29 @@
         <v>13</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" s="21" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="36" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B7" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -2671,95 +2686,95 @@
         <v>15</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A9" s="36" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B9" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B10" s="21" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="36" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B11" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="36" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B12" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="36" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B13" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="37" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B14" s="21" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="36" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B15" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="36" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B16" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -2770,51 +2785,51 @@
         <v>19</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="36" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B18" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="36" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B19" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C19" s="21" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="37" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="36" t="s">
+      <c r="B20" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="21" t="s">
         <v>191</v>
-      </c>
-      <c r="B20" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="21" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="37" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B21" s="21" t="s">
         <v>19</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -2825,37 +2840,37 @@
         <v>19</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="36" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B23" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A24" s="35" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="27" x14ac:dyDescent="0.3">
       <c r="A25" s="27" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B25" t="s">
         <v>13</v>
       </c>
       <c r="C25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D25" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -2868,7 +2883,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.88671875" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2955,17 +2970,21 @@
     </row>
     <row r="8" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
     </row>
     <row r="9" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
+      <c r="A9" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>212</v>
+      </c>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
     </row>
@@ -3040,6 +3059,7 @@
     <hyperlink ref="A6" r:id="rId1"/>
     <hyperlink ref="A7" r:id="rId2"/>
     <hyperlink ref="A8" r:id="rId3"/>
+    <hyperlink ref="A9" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3047,27 +3067,30 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.88671875" customWidth="1"/>
-    <col min="2" max="2" width="100" customWidth="1"/>
-    <col min="3" max="4" width="17.109375" style="21"/>
+    <col min="2" max="2" width="36.44140625" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.109375" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="13" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>45</v>
+        <v>213</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="C1" s="21"/>
+        <v>64</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>209</v>
+      </c>
       <c r="D1" s="21"/>
       <c r="E1" s="15"/>
     </row>
@@ -3076,7 +3099,10 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3084,7 +3110,10 @@
         <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>46</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3092,26 +3121,54 @@
         <v>34</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>68</v>
+        <v>67</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B6" t="s">
-        <v>202</v>
+        <v>201</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>196</v>
+      </c>
+      <c r="B7" t="s">
+        <v>208</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>211</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C6" r:id="rId5"/>
+    <hyperlink ref="C7" r:id="rId6"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Example_Profile.xlsx and ex02.xml
</commit_message>
<xml_diff>
--- a/examples/Example_Profile.xlsx
+++ b/examples/Example_Profile.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="480" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="480" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="STIX Package" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="STIX Header" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="TTP" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Indicator" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Namespaces" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="Instance Mapping" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Overview" sheetId="1" r:id="rId1"/>
+    <sheet name="STIX Package" sheetId="2" r:id="rId2"/>
+    <sheet name="STIX Header" sheetId="3" r:id="rId3"/>
+    <sheet name="TTP" sheetId="4" r:id="rId4"/>
+    <sheet name="Indicator" sheetId="5" r:id="rId5"/>
+    <sheet name="Namespaces" sheetId="6" r:id="rId6"/>
+    <sheet name="Instance Mapping" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="145621" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -449,9 +448,6 @@
     <t>stix:STIXPackageVersionEnum</t>
   </si>
   <si>
-    <t>1.0.1, 1.1</t>
-  </si>
-  <si>
     <t>TTPsType</t>
   </si>
   <si>
@@ -660,17 +656,16 @@
   </si>
   <si>
     <t>stix:Indicator</t>
+  </si>
+  <si>
+    <t>1.0.1, 1.1, 1.1.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="@" numFmtId="165"/>
-  </numFmts>
-  <fonts count="22">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -679,22 +674,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="15"/>
       <color rgb="FF1F497D"/>
       <name val="Calibri"/>
@@ -702,7 +682,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="15"/>
       <color rgb="FF1F497D"/>
       <name val="Calibri"/>
@@ -717,7 +697,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -739,14 +719,14 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="1"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -761,7 +741,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -796,7 +776,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
@@ -811,7 +791,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
@@ -819,7 +799,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
@@ -866,14 +846,14 @@
     </fill>
   </fills>
   <borders count="8">
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -882,7 +862,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top style="thick">
@@ -891,21 +871,25 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
-      <top style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left style="medium">
         <color rgb="FFDDDDDD"/>
       </left>
@@ -916,14 +900,18 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thin"/>
-      <right style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left style="medium">
         <color rgb="FFDDDDDD"/>
       </left>
@@ -935,198 +923,69 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="21" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="4" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="2" fontId="8" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="3" fontId="9" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="4" fontId="19" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
+  <cellStyleXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="33">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="16" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="4" numFmtId="164" xfId="21">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="7" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="2" fontId="8" numFmtId="164" xfId="22">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="3" fontId="9" numFmtId="164" xfId="23">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="10" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="11" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="12" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="13" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="14" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="15" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="16" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="5" fontId="17" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="0" fontId="6" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="4" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="4" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="4" numFmtId="165" xfId="21">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="0" fontId="4" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="5" fillId="6" fontId="18" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="6" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="4" fontId="19" numFmtId="165" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="6" fillId="3" fontId="9" numFmtId="165" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="0" fontId="6" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="3" fontId="9" numFmtId="165" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="7" fillId="6" fontId="18" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="7" fillId="4" fontId="19" numFmtId="164" xfId="24">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="7" fillId="3" fontId="9" numFmtId="164" xfId="23">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="20" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="21" numFmtId="164" xfId="20">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="11">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Heading 1" xfId="21"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Good" xfId="22"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Bad" xfId="23"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Neutral" xfId="24"/>
-    <cellStyle builtinId="8" customBuiltin="false" name="*unknown*" xfId="20"/>
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="TableStyleLight1" xfId="2"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1185,32 +1044,327 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF1F497D"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C24" activeCellId="0" pane="topLeft" sqref="C24"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="67.6683673469388"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.5561224489796"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.1020408163265"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+    <col min="1" max="1" width="67.6640625"/>
+    <col min="2" max="2" width="34.5546875"/>
+    <col min="3" max="3" width="38.109375"/>
+    <col min="4" max="4" width="43.6640625"/>
+    <col min="5" max="1025" width="8.5546875"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="20.25" outlineLevel="0" r="1">
+    <row r="1" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1226,7 +1380,7 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="18" outlineLevel="0" r="2">
+    <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -1242,7 +1396,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.4" outlineLevel="0" r="3">
+    <row r="3" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>8</v>
       </c>
@@ -1258,7 +1412,7 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="4">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>12</v>
       </c>
@@ -1274,7 +1428,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.4" outlineLevel="0" r="5">
+    <row r="5" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
@@ -1288,7 +1442,7 @@
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.4" outlineLevel="0" r="6">
+    <row r="6" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>19</v>
       </c>
@@ -1304,7 +1458,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.4" outlineLevel="0" r="7">
+    <row r="7" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>23</v>
       </c>
@@ -1320,7 +1474,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.4" outlineLevel="0" r="8">
+    <row r="8" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="11"/>
       <c r="B8" s="7" t="s">
         <v>27</v>
@@ -1334,7 +1488,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.4" outlineLevel="0" r="9">
+    <row r="9" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="11"/>
       <c r="B9" s="7" t="s">
         <v>30</v>
@@ -1348,7 +1502,7 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.4" outlineLevel="0" r="10">
+    <row r="10" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="14"/>
       <c r="C10" s="12" t="s">
@@ -1360,7 +1514,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="20.4" outlineLevel="0" r="11">
+    <row r="11" spans="1:6" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A11" s="4"/>
       <c r="B11" s="2" t="s">
         <v>34</v>
@@ -1372,7 +1526,7 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="12">
+    <row r="12" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="14"/>
       <c r="C12" s="7" t="s">
@@ -1381,7 +1535,7 @@
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="20.4" outlineLevel="0" r="13">
+    <row r="13" spans="1:6" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A13" s="4"/>
       <c r="B13" s="2" t="s">
         <v>37</v>
@@ -1392,7 +1546,7 @@
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="14">
+    <row r="14" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="14"/>
       <c r="C14" s="6" t="s">
@@ -1401,7 +1555,7 @@
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="20.4" outlineLevel="0" r="15">
+    <row r="15" spans="1:6" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A15" s="4"/>
       <c r="B15" s="2" t="s">
         <v>40</v>
@@ -1412,7 +1566,7 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="16">
+    <row r="16" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="14"/>
       <c r="C16" s="7" t="s">
@@ -1421,7 +1575,7 @@
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="20.4" outlineLevel="0" r="17">
+    <row r="17" spans="1:6" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A17" s="4"/>
       <c r="B17" s="2" t="s">
         <v>43</v>
@@ -1432,7 +1586,7 @@
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="18">
+    <row r="18" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="6" t="s">
         <v>45</v>
@@ -1443,7 +1597,7 @@
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.4" outlineLevel="0" r="19">
+    <row r="19" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="6" t="s">
         <v>47</v>
@@ -1454,7 +1608,7 @@
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.4" outlineLevel="0" r="20">
+    <row r="20" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="14"/>
       <c r="C20" s="7" t="s">
@@ -1463,7 +1617,7 @@
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.8" outlineLevel="0" r="21">
+    <row r="21" spans="1:6" ht="16.8" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B21" s="2" t="s">
         <v>50</v>
       </c>
@@ -1471,330 +1625,322 @@
         <v>51</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="22">
+    <row r="22" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C22" s="7" t="s">
         <v>52</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="23">
+    <row r="23" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C23" s="7" t="s">
         <v>53</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="24">
+    <row r="24" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C24" s="12" t="s">
         <v>54</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="25">
+    <row r="25" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C25" s="12" t="s">
         <v>55</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="26">
+    <row r="26" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C26" s="12" t="s">
         <v>56</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="27">
+    <row r="27" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C27" s="12" t="s">
         <v>57</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="28">
+    <row r="28" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C28" s="7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="29">
+    <row r="29" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C29" s="7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="30">
+    <row r="30" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C30" s="7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="31">
+    <row r="31" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C31" s="7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="32">
+    <row r="32" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C32" s="7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="33">
+    <row r="33" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C33" s="7" t="s">
         <v>63</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="34">
+    <row r="34" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C34" s="12" t="s">
         <v>64</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="35">
+    <row r="35" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C35" s="7" t="s">
         <v>65</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="36">
+    <row r="36" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C36" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="37">
+    <row r="37" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C37" s="7" t="s">
         <v>67</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="38">
+    <row r="38" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C38" s="12" t="s">
         <v>68</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="39">
+    <row r="39" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C39" s="12" t="s">
         <v>69</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="40">
+    <row r="40" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C40" s="12" t="s">
         <v>70</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="41">
+    <row r="41" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C41" s="7" t="s">
         <v>71</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="42">
+    <row r="42" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C42" s="7" t="s">
         <v>72</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="43">
+    <row r="43" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C43" s="7" t="s">
         <v>73</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="44">
+    <row r="44" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C44" s="7" t="s">
         <v>74</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="45">
+    <row r="45" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C45" s="7" t="s">
         <v>75</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="46">
+    <row r="46" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C46" s="7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="47">
+    <row r="47" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C47" s="7" t="s">
         <v>77</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="48">
+    <row r="48" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C48" s="7" t="s">
         <v>78</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="49">
+    <row r="49" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C49" s="7" t="s">
         <v>79</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="50">
+    <row r="50" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C50" s="7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="51">
+    <row r="51" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C51" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="52">
+    <row r="52" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C52" s="7" t="s">
         <v>82</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="53">
+    <row r="53" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C53" s="7" t="s">
         <v>83</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="54">
+    <row r="54" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C54" s="7" t="s">
         <v>84</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="55">
+    <row r="55" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C55" s="7" t="s">
         <v>85</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="56">
+    <row r="56" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C56" s="7" t="s">
         <v>86</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="57">
+    <row r="57" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C57" s="7" t="s">
         <v>87</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="58">
+    <row r="58" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C58" s="7" t="s">
         <v>88</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="59">
+    <row r="59" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C59" s="7" t="s">
         <v>89</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="60">
+    <row r="60" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C60" s="7" t="s">
         <v>90</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="61">
+    <row r="61" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C61" s="7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="62">
+    <row r="62" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C62" s="7" t="s">
         <v>92</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="63">
+    <row r="63" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C63" s="7" t="s">
         <v>93</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="64">
+    <row r="64" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C64" s="7" t="s">
         <v>94</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="65">
+    <row r="65" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C65" s="7" t="s">
         <v>95</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="66">
+    <row r="66" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C66" s="7" t="s">
         <v>96</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="67">
+    <row r="67" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C67" s="7" t="s">
         <v>97</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="68">
+    <row r="68" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C68" s="7" t="s">
         <v>98</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="69">
+    <row r="69" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C69" s="12" t="s">
         <v>99</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="70">
+    <row r="70" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C70" s="7" t="s">
         <v>100</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="71">
+    <row r="71" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C71" s="7" t="s">
         <v>101</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="72">
+    <row r="72" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C72" s="7" t="s">
         <v>102</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="73">
+    <row r="73" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C73" s="7" t="s">
         <v>103</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="74">
+    <row r="74" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C74" s="7" t="s">
         <v>104</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="75">
+    <row r="75" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C75" s="7" t="s">
         <v>105</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="76">
+    <row r="76" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C76" s="7" t="s">
         <v>106</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="77">
+    <row r="77" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C77" s="7" t="s">
         <v>107</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="78">
+    <row r="78" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C78" s="7" t="s">
         <v>108</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="79">
+    <row r="79" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C79" s="7" t="s">
         <v>109</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:F17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100">
-      <selection activeCell="B6" activeCellId="0" pane="topLeft" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="16" width="57.5612244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="17" width="14.3367346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="17" width="27"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="17" width="46.3316326530612"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="17" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="17" width="9.43877551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col min="1" max="1" width="57.5546875" style="16"/>
+    <col min="2" max="2" width="14.33203125" style="17"/>
+    <col min="3" max="3" width="27" style="17"/>
+    <col min="4" max="4" width="46.33203125" style="17"/>
+    <col min="5" max="5" width="12.5546875" style="17"/>
+    <col min="6" max="6" width="9.44140625" style="17"/>
+    <col min="7" max="1025" width="8.5546875"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="19.5" outlineLevel="0" r="1" s="21">
+    <row r="1" spans="1:6" s="21" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="18" t="s">
         <v>110</v>
       </c>
@@ -1812,189 +1958,189 @@
       </c>
       <c r="F1" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="2">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>115</v>
       </c>
       <c r="B2" s="23"/>
-      <c r="C2" s="0"/>
+      <c r="C2"/>
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
       <c r="F2" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="3">
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>116</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" t="s">
         <v>118</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="4">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="24" t="s">
         <v>119</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" t="s">
         <v>121</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="5">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
         <v>122</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" t="s">
         <v>123</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="6">
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
         <v>124</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" t="s">
         <v>125</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="7">
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="25" t="s">
         <v>126</v>
       </c>
       <c r="B7" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" t="s">
         <v>128</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="8">
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="25" t="s">
         <v>129</v>
       </c>
       <c r="B8" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" t="s">
         <v>130</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="9">
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="24" t="s">
         <v>131</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" t="s">
         <v>132</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="10">
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="27" t="s">
         <v>133</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" t="s">
         <v>134</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="11">
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="27" t="s">
         <v>135</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" t="s">
         <v>136</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="12">
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>137</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" t="s">
         <v>138</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="13">
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
         <v>139</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" t="s">
         <v>138</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="14">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>140</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" t="s">
         <v>141</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="22" t="s">
         <v>142</v>
-      </c>
-      <c r="F14" s="4"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="15">
-      <c r="A15" s="22" t="s">
-        <v>143</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -2002,7 +2148,7 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="16">
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
         <v>13</v>
       </c>
@@ -2010,50 +2156,38 @@
         <v>120</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.4" outlineLevel="0" r="17"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.4" outlineLevel="0" r="18"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.4" outlineLevel="0" r="19"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.4" outlineLevel="0" r="20"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100">
-      <selection activeCell="D4" activeCellId="0" pane="topLeft" sqref="D4"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="16" width="57.5612244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="17" width="14.3367346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="17" width="38.219387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="17" width="78"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="17" width="21.5561224489796"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="17" width="9.43877551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col min="1" max="1" width="57.5546875" style="16"/>
+    <col min="2" max="2" width="14.33203125" style="17"/>
+    <col min="3" max="3" width="38.21875" style="17"/>
+    <col min="4" max="4" width="78" style="17"/>
+    <col min="5" max="5" width="21.5546875" style="17"/>
+    <col min="6" max="6" width="9.44140625" style="17"/>
+    <col min="7" max="1025" width="8.5546875"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="19.5" outlineLevel="0" r="1" s="21">
+    <row r="1" spans="1:6" s="21" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="18" t="s">
         <v>110</v>
       </c>
@@ -2071,9 +2205,9 @@
       </c>
       <c r="F1" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="2">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
@@ -2081,114 +2215,106 @@
       <c r="E2" s="23"/>
       <c r="F2" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.4" outlineLevel="0" r="3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>147</v>
+      <c r="C3" t="s">
+        <v>146</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.55" outlineLevel="0" r="4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" t="s">
+        <v>148</v>
+      </c>
+      <c r="D4" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="E4" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="24" t="s">
         <v>151</v>
-      </c>
-      <c r="F4" s="4"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.4" outlineLevel="0" r="5">
-      <c r="A5" s="24" t="s">
-        <v>152</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>153</v>
+      <c r="C5" t="s">
+        <v>152</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.4" outlineLevel="0" r="6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>155</v>
+      <c r="C6" t="s">
+        <v>154</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.4" outlineLevel="0" r="7">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>157</v>
+      <c r="C7" t="s">
+        <v>156</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100">
-      <selection activeCell="B3" activeCellId="0" pane="topLeft" sqref="B3"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="16" width="57.5612244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="17" width="14.3367346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="17" width="7.66836734693878"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="17" width="46.3316326530612"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="17" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="17" width="9.43877551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col min="1" max="1" width="57.5546875" style="16"/>
+    <col min="2" max="2" width="14.33203125" style="17"/>
+    <col min="3" max="3" width="7.6640625" style="17"/>
+    <col min="4" max="4" width="46.33203125" style="17"/>
+    <col min="5" max="5" width="12.5546875" style="17"/>
+    <col min="6" max="6" width="9.44140625" style="17"/>
+    <col min="7" max="1025" width="8.5546875"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="19.5" outlineLevel="0" r="1" s="21">
+    <row r="1" spans="1:6" s="21" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="18" t="s">
         <v>110</v>
       </c>
@@ -2206,7 +2332,7 @@
       </c>
       <c r="F1" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="2">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>13</v>
       </c>
@@ -2216,53 +2342,45 @@
       <c r="E2" s="23"/>
       <c r="F2" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="B3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C3" t="s">
         <v>146</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="D3" s="0"/>
-      <c r="E3" s="0"/>
-      <c r="F3" s="0"/>
+      <c r="D3"/>
+      <c r="E3"/>
+      <c r="F3"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100">
-      <selection activeCell="A12" activeCellId="0" pane="topLeft" sqref="A12"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.1020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3367346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.219387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="52.4387755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
+    <col min="1" max="1" width="55.109375"/>
+    <col min="2" max="2" width="14.33203125"/>
+    <col min="3" max="3" width="38.21875"/>
+    <col min="4" max="4" width="52.44140625"/>
+    <col min="5" max="5" width="10.6640625"/>
+    <col min="6" max="1025" width="8.5546875"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="19.5" outlineLevel="0" r="1" s="21">
+    <row r="1" spans="1:6" s="21" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="18" t="s">
         <v>110</v>
       </c>
@@ -2280,526 +2398,494 @@
       </c>
       <c r="F1" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.4" outlineLevel="0" r="2">
+    <row r="2" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>117</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" t="s">
         <v>138</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.4" outlineLevel="0" r="4">
+    <row r="4" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
         <v>139</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>120</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" t="s">
         <v>138</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.4" outlineLevel="0" r="5">
+    <row r="5" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="B5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C5" t="s">
         <v>146</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="6">
+    </row>
+    <row r="6" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>117</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="7">
+      <c r="C6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
+        <v>158</v>
+      </c>
+      <c r="B7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A8" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="B8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
         <v>159</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B9" t="s">
         <v>120</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="8">
-      <c r="A8" s="29" t="s">
-        <v>152</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.4" outlineLevel="0" r="9">
-      <c r="A9" s="29" t="s">
+      <c r="C9" t="s">
         <v>160</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="10">
+    </row>
+    <row r="10" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" t="s">
         <v>117</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A11" s="29" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="11">
-      <c r="A11" s="29" t="s">
+      <c r="B11" t="s">
+        <v>120</v>
+      </c>
+      <c r="C11" t="s">
         <v>163</v>
       </c>
-      <c r="B11" s="0" t="s">
+    </row>
+    <row r="12" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A12" s="29" t="s">
+        <v>164</v>
+      </c>
+      <c r="B12" t="s">
         <v>120</v>
       </c>
-      <c r="C11" s="0" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="12">
-      <c r="A12" s="29" t="s">
+      <c r="C12" t="s">
         <v>165</v>
       </c>
-      <c r="B12" s="0" t="s">
+    </row>
+    <row r="13" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A13" s="29" t="s">
+        <v>166</v>
+      </c>
+      <c r="B13" t="s">
         <v>120</v>
       </c>
-      <c r="C12" s="0" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="13">
-      <c r="A13" s="29" t="s">
+      <c r="C13" t="s">
         <v>167</v>
       </c>
-      <c r="B13" s="0" t="s">
+    </row>
+    <row r="14" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A14" s="30" t="s">
+        <v>168</v>
+      </c>
+      <c r="B14" t="s">
+        <v>127</v>
+      </c>
+      <c r="C14" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A15" s="29" t="s">
+        <v>170</v>
+      </c>
+      <c r="B15" t="s">
         <v>120</v>
       </c>
-      <c r="C13" s="0" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="14">
-      <c r="A14" s="30" t="s">
-        <v>169</v>
-      </c>
-      <c r="B14" s="0" t="s">
+      <c r="C15" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A16" s="29" t="s">
+        <v>172</v>
+      </c>
+      <c r="B16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C16" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A17" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="B17" t="s">
         <v>127</v>
       </c>
-      <c r="C14" s="0" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="15">
-      <c r="A15" s="29" t="s">
-        <v>171</v>
-      </c>
-      <c r="B15" s="0" t="s">
+      <c r="C17" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A18" s="29" t="s">
+        <v>174</v>
+      </c>
+      <c r="B18" t="s">
         <v>120</v>
       </c>
-      <c r="C15" s="0" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="16">
-      <c r="A16" s="29" t="s">
-        <v>173</v>
-      </c>
-      <c r="B16" s="0" t="s">
+      <c r="C18" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A19" s="29" t="s">
+        <v>176</v>
+      </c>
+      <c r="B19" t="s">
         <v>120</v>
       </c>
-      <c r="C16" s="0" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="17">
-      <c r="A17" s="30" t="s">
-        <v>154</v>
-      </c>
-      <c r="B17" s="0" t="s">
+      <c r="C19" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A20" s="30" t="s">
+        <v>178</v>
+      </c>
+      <c r="B20" t="s">
         <v>127</v>
       </c>
-      <c r="C17" s="0" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="18">
-      <c r="A18" s="29" t="s">
-        <v>175</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="19">
-      <c r="A19" s="29" t="s">
-        <v>177</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="20">
-      <c r="A20" s="30" t="s">
+      <c r="C20" t="s">
         <v>179</v>
       </c>
-      <c r="B20" s="0" t="s">
+    </row>
+    <row r="21" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A21" s="30" t="s">
+        <v>180</v>
+      </c>
+      <c r="B21" t="s">
         <v>127</v>
       </c>
-      <c r="C20" s="0" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="21">
-      <c r="A21" s="30" t="s">
-        <v>181</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="22">
+      <c r="C21" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A22" s="30" t="s">
         <v>140</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" t="s">
         <v>127</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A23" s="29" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="23">
-      <c r="A23" s="29" t="s">
+      <c r="B23" t="s">
+        <v>120</v>
+      </c>
+      <c r="C23" t="s">
         <v>183</v>
       </c>
-      <c r="B23" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="C23" s="0" t="s">
+    </row>
+    <row r="24" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A24" s="28" t="s">
         <v>184</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="24">
-      <c r="A24" s="28" t="s">
+    <row r="25" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A25" s="15" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="27" outlineLevel="0" r="25">
-      <c r="A25" s="15" t="s">
+      <c r="B25" t="s">
+        <v>117</v>
+      </c>
+      <c r="C25" t="s">
         <v>186</v>
       </c>
-      <c r="B25" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="C25" s="0" t="s">
+      <c r="D25" t="s">
         <v>187</v>
       </c>
-      <c r="D25" s="0" t="s">
-        <v>188</v>
-      </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:F11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B10" activeCellId="0" pane="topLeft" sqref="B10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.8877551020408"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.8877551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.89285714285714"/>
+    <col min="1" max="1" width="47.88671875"/>
+    <col min="2" max="2" width="27.88671875"/>
+    <col min="3" max="1025" width="9.88671875"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="19.5" outlineLevel="0" r="1" s="21">
+    <row r="1" spans="1:6" s="21" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="B1" s="19" t="s">
         <v>189</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="C1"/>
+      <c r="D1"/>
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="31" t="str">
+        <f>HYPERLINK("http://www.w3.org/2001/XMLSchema-instance","http://www.w3.org/2001/XMLSchema-instance")</f>
+        <v>http://www.w3.org/2001/XMLSchema-instance</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>190</v>
-      </c>
-      <c r="C1" s="0"/>
-      <c r="D1" s="0"/>
-      <c r="E1" s="4"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="2">
-      <c r="A2" s="31" t="str">
-        <f aca="false">HYPERLINK("http://www.w3.org/2001/XMLSchema-instance","http://www.w3.org/2001/XMLSchema-instance")</f>
-        <v>http://www.w3.org/2001/XMLSchema-instance</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>191</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.4" outlineLevel="0" r="3">
+    <row r="3" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="str">
-        <f aca="false">HYPERLINK("http://stix.mitre.org/stix-1","http://stix.mitre.org/stix-1")</f>
+        <f>HYPERLINK("http://stix.mitre.org/stix-1","http://stix.mitre.org/stix-1")</f>
         <v>http://stix.mitre.org/stix-1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.4" outlineLevel="0" r="4">
+    <row r="4" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="31" t="str">
-        <f aca="false">HYPERLINK("http://stix.mitre.org/common-1","http://stix.mitre.org/common-1")</f>
+        <f>HYPERLINK("http://stix.mitre.org/common-1","http://stix.mitre.org/common-1")</f>
         <v>http://stix.mitre.org/common-1</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.4" outlineLevel="0" r="5">
+    <row r="5" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="31" t="str">
-        <f aca="false">HYPERLINK("http://stix.mitre.org/default_vocabularies-1","http://stix.mitre.org/default_vocabularies-1")</f>
+        <f>HYPERLINK("http://stix.mitre.org/default_vocabularies-1","http://stix.mitre.org/default_vocabularies-1")</f>
         <v>http://stix.mitre.org/default_vocabularies-1</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.4" outlineLevel="0" r="6">
+    <row r="6" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>195</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>196</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.4" outlineLevel="0" r="7">
+    <row r="7" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>197</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>198</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.4" outlineLevel="0" r="8">
+    <row r="8" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="32" t="s">
+        <v>198</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>199</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>200</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.4" outlineLevel="0" r="9">
+    <row r="9" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="32" t="s">
+        <v>200</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>201</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>202</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="10"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.4" outlineLevel="0" r="11"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.4" outlineLevel="0" r="12"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.4" outlineLevel="0" r="13"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.4" outlineLevel="0" r="14"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.4" outlineLevel="0" r="15"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.4" outlineLevel="0" r="16"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.4" outlineLevel="0" r="17"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.4" outlineLevel="0" r="18"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.4" outlineLevel="0" r="19"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.4" outlineLevel="0" r="20"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="http://stix.mitre.org/TTP-1" ref="A6" r:id="rId1"/>
-    <hyperlink display="http://stix.mitre.org/Incident-1" ref="A7" r:id="rId2"/>
-    <hyperlink display="http://cybox.mitre.org/cybox-2" ref="A8" r:id="rId3"/>
-    <hyperlink display="http://stix.mitre.org/Indicator-2" ref="A9" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId1"/>
+    <hyperlink ref="A7" r:id="rId2"/>
+    <hyperlink ref="A8" r:id="rId3"/>
+    <hyperlink ref="A9" r:id="rId4"/>
   </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A13" activeCellId="0" pane="topLeft" sqref="A13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.8928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.4489795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.6683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="17.1071428571429"/>
+    <col min="1" max="1" width="33.88671875"/>
+    <col min="2" max="2" width="36.44140625"/>
+    <col min="3" max="3" width="25.6640625"/>
+    <col min="4" max="1025" width="17.109375"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="19.5" outlineLevel="0" r="1" s="21">
+    <row r="1" spans="1:5" s="21" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="B1" s="19" t="s">
         <v>203</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="C1" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="D1"/>
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" t="s">
         <v>205</v>
       </c>
-      <c r="D1" s="0"/>
-      <c r="E1" s="4"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="2">
-      <c r="A2" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="32" t="s">
         <v>206</v>
       </c>
-      <c r="C2" s="32" t="s">
+    </row>
+    <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B3" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="3">
-      <c r="A3" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="B3" s="0" t="s">
+      <c r="C3" s="32" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
         <v>208</v>
       </c>
-      <c r="C3" s="32" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="4">
-      <c r="A4" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="0" t="s">
+      <c r="C4" s="32" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B5" t="s">
         <v>209</v>
       </c>
-      <c r="C4" s="32" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="5">
-      <c r="A5" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="B5" s="0" t="s">
+      <c r="C5" s="32" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>184</v>
+      </c>
+      <c r="B6" t="s">
         <v>210</v>
       </c>
-      <c r="C5" s="32" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="6">
-      <c r="A6" s="0" t="s">
-        <v>185</v>
-      </c>
-      <c r="B6" s="0" t="s">
+      <c r="C6" s="32" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>157</v>
+      </c>
+      <c r="B7" t="s">
         <v>211</v>
       </c>
-      <c r="C6" s="32" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="7">
-      <c r="A7" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>212</v>
-      </c>
       <c r="C7" s="32" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="http://stix.mitre.org/stix-1" ref="C2" r:id="rId1"/>
-    <hyperlink display="http://stix.mitre.org/stix-1" ref="C3" r:id="rId2"/>
-    <hyperlink display="http://stix.mitre.org/TTP-1" ref="C4" r:id="rId3"/>
-    <hyperlink display="http://stix.mitre.org/stix-1" ref="C5" r:id="rId4"/>
-    <hyperlink display="http://cybox.mitre.org/cybox-2" ref="C6" r:id="rId5"/>
-    <hyperlink display="http://stix.mitre.org/Indicator-2" ref="C7" r:id="rId6"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C6" r:id="rId5"/>
+    <hyperlink ref="C7" r:id="rId6"/>
   </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
edit example profile to cover rfc as labels
</commit_message>
<xml_diff>
--- a/examples/Example_Profile.xlsx
+++ b/examples/Example_Profile.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="218">
   <si>
     <t>Profile Information</t>
   </si>
@@ -659,13 +659,28 @@
   </si>
   <si>
     <t>1.0.1, 1.1, 1.1.1</t>
+  </si>
+  <si>
+    <t>MUST</t>
+  </si>
+  <si>
+    <t>SHOULD</t>
+  </si>
+  <si>
+    <t>MAY</t>
+  </si>
+  <si>
+    <t>MUST NOT</t>
+  </si>
+  <si>
+    <t>AKA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -806,6 +821,13 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -928,7 +950,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -978,6 +1000,7 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1351,8 +1374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1455,7 +1478,9 @@
       <c r="D6" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="4"/>
+      <c r="E6" s="33" t="s">
+        <v>217</v>
+      </c>
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
@@ -1471,7 +1496,9 @@
       <c r="D7" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="4"/>
+      <c r="E7" s="15" t="s">
+        <v>213</v>
+      </c>
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
@@ -1485,7 +1512,9 @@
       <c r="D8" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="4"/>
+      <c r="E8" s="10" t="s">
+        <v>214</v>
+      </c>
       <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
@@ -1499,7 +1528,9 @@
       <c r="D9" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="4"/>
+      <c r="E9" s="13" t="s">
+        <v>215</v>
+      </c>
       <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
@@ -1511,7 +1542,9 @@
       <c r="D10" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="4"/>
+      <c r="E10" s="12" t="s">
+        <v>216</v>
+      </c>
       <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" ht="19.8" x14ac:dyDescent="0.4">
@@ -1917,7 +1950,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1926,7 +1959,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1973,7 +2006,7 @@
         <v>116</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>117</v>
+        <v>213</v>
       </c>
       <c r="C3" t="s">
         <v>118</v>
@@ -2001,7 +2034,7 @@
         <v>122</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>117</v>
+        <v>213</v>
       </c>
       <c r="C5" t="s">
         <v>123</v>
@@ -2029,7 +2062,7 @@
         <v>126</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>127</v>
+        <v>216</v>
       </c>
       <c r="C7" t="s">
         <v>128</v>
@@ -2043,7 +2076,7 @@
         <v>129</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>127</v>
+        <v>216</v>
       </c>
       <c r="C8" t="s">
         <v>130</v>
@@ -2071,7 +2104,7 @@
         <v>133</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>127</v>
+        <v>216</v>
       </c>
       <c r="C10" t="s">
         <v>134</v>
@@ -2085,7 +2118,7 @@
         <v>135</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>127</v>
+        <v>216</v>
       </c>
       <c r="C11" t="s">
         <v>136</v>
@@ -2099,7 +2132,7 @@
         <v>137</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>117</v>
+        <v>213</v>
       </c>
       <c r="C12" t="s">
         <v>138</v>
@@ -2127,7 +2160,7 @@
         <v>140</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>117</v>
+        <v>213</v>
       </c>
       <c r="C14" t="s">
         <v>141</v>

</xml_diff>

<commit_message>
further testing for MUST and MUST NOT keywords
</commit_message>
<xml_diff>
--- a/examples/Example_Profile.xlsx
+++ b/examples/Example_Profile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="480" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="480" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -1958,7 +1958,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -2399,8 +2399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2463,7 +2463,7 @@
         <v>145</v>
       </c>
       <c r="B5" t="s">
-        <v>117</v>
+        <v>213</v>
       </c>
       <c r="C5" t="s">
         <v>146</v>
@@ -2595,7 +2595,7 @@
         <v>153</v>
       </c>
       <c r="B17" t="s">
-        <v>127</v>
+        <v>216</v>
       </c>
       <c r="C17" t="s">
         <v>154</v>

</xml_diff>

<commit_message>
Updated examples to align with validation options
</commit_message>
<xml_diff>
--- a/examples/Example_Profile.xlsx
+++ b/examples/Example_Profile.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="480" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="480" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="Overview" sheetId="1" r:id="rId1"/>
-    <sheet name="STIX Package" sheetId="2" r:id="rId2"/>
-    <sheet name="STIX Header" sheetId="3" r:id="rId3"/>
-    <sheet name="TTP" sheetId="4" r:id="rId4"/>
-    <sheet name="Indicator" sheetId="5" r:id="rId5"/>
-    <sheet name="Namespaces" sheetId="6" r:id="rId6"/>
-    <sheet name="Instance Mapping" sheetId="7" r:id="rId7"/>
+    <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="STIX Package" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="STIX Header" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="TTP" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Indicator" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Namespaces" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Instance Mapping" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="145621" iterateDelta="1E-4"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
@@ -448,6 +449,9 @@
     <t>stix:STIXPackageVersionEnum</t>
   </si>
   <si>
+    <t>1.0.1, 1.1, 1.1.1</t>
+  </si>
+  <si>
     <t>TTPsType</t>
   </si>
   <si>
@@ -472,7 +476,7 @@
     <t>stixVocabs:PackageIntentVocab-1.0</t>
   </si>
   <si>
-    <t>Indicators - Phishing</t>
+    <t>Indicators - Phishing, Indicators</t>
   </si>
   <si>
     <t>Description</t>
@@ -583,7 +587,7 @@
     <t>cybox:ObjectPropertiesType</t>
   </si>
   <si>
-    <t>FileObj:FileObjectType, AddressObject:AddressObjectType, EmailMessageObj:EmailMessageObjectType</t>
+    <t>DomainNameObj:DomainNameObjectType, FileObj:FileObjectType, AddressObject:AddressObjectType, EmailMessageObj:EmailMessageObjectType</t>
   </si>
   <si>
     <t>Namespace</t>
@@ -656,16 +660,17 @@
   </si>
   <si>
     <t>stix:Indicator</t>
-  </si>
-  <si>
-    <t>1.0.1, 1.1, 1.1.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="165" formatCode="@"/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -674,7 +679,29 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="15"/>
       <color rgb="FF1F497D"/>
       <name val="Calibri"/>
@@ -682,7 +709,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <b val="true"/>
       <sz val="15"/>
       <color rgb="FF1F497D"/>
       <name val="Calibri"/>
@@ -697,7 +724,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <b val="true"/>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -719,14 +746,14 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <b val="true"/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="1"/>
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <b val="true"/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -741,7 +768,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -776,7 +803,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <b val="true"/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
@@ -784,14 +811,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <u/>
+      <u val="single"/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
@@ -799,7 +819,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <u/>
+      <u val="single"/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
@@ -816,6 +836,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor rgb="FFDDDDDD"/>
       </patternFill>
@@ -824,12 +850,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
     <fill>
@@ -845,15 +865,15 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
-    <border>
+  <borders count="9">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -862,7 +882,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top style="thick">
@@ -871,25 +891,21 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
+      <top style="thin"/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="medium">
         <color rgb="FFDDDDDD"/>
       </left>
@@ -900,18 +916,21 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="medium">
         <color rgb="FFDDDDDD"/>
       </left>
@@ -923,69 +942,183 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0"/>
+  <cellStyleXfs count="22">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="33">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="16" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="6" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="6" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="8" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="8" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="TableStyleLight1" xfId="2"/>
+  <cellStyles count="8">
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1044,327 +1177,33 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF1F497D"/>
       <rgbColor rgb="FF333333"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="1F497D"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="EEECE1"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4F81BD"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="C0504D"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="9BBB59"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8064A2"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4BACC6"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="F79646"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000FF"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="800080"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <tabColor rgb="00FFFFFF"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C24" activeCellId="1" sqref="A22 C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="67.6640625"/>
-    <col min="2" max="2" width="34.5546875"/>
-    <col min="3" max="3" width="38.109375"/>
-    <col min="4" max="4" width="43.6640625"/>
-    <col min="5" max="1025" width="8.5546875"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="67.6683673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.5561224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.1020408163265"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.55612244897959"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1380,7 +1219,7 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -1396,7 +1235,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
         <v>8</v>
       </c>
@@ -1412,7 +1251,7 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="s">
         <v>12</v>
       </c>
@@ -1428,7 +1267,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
@@ -1442,7 +1281,7 @@
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="s">
         <v>19</v>
       </c>
@@ -1458,7 +1297,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="11" t="s">
         <v>23</v>
       </c>
@@ -1474,7 +1313,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="11"/>
       <c r="B8" s="7" t="s">
         <v>27</v>
@@ -1488,7 +1327,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="11"/>
       <c r="B9" s="7" t="s">
         <v>30</v>
@@ -1502,7 +1341,7 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4"/>
       <c r="B10" s="14"/>
       <c r="C10" s="12" t="s">
@@ -1514,7 +1353,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:6" ht="19.8" x14ac:dyDescent="0.4">
+    <row r="11" customFormat="false" ht="19.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4"/>
       <c r="B11" s="2" t="s">
         <v>34</v>
@@ -1526,7 +1365,7 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4"/>
       <c r="B12" s="14"/>
       <c r="C12" s="7" t="s">
@@ -1535,7 +1374,7 @@
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:6" ht="19.8" x14ac:dyDescent="0.4">
+    <row r="13" customFormat="false" ht="19.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4"/>
       <c r="B13" s="2" t="s">
         <v>37</v>
@@ -1546,7 +1385,7 @@
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4"/>
       <c r="B14" s="14"/>
       <c r="C14" s="6" t="s">
@@ -1555,7 +1394,7 @@
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" ht="19.8" x14ac:dyDescent="0.4">
+    <row r="15" customFormat="false" ht="19.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4"/>
       <c r="B15" s="2" t="s">
         <v>40</v>
@@ -1566,7 +1405,7 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4"/>
       <c r="B16" s="14"/>
       <c r="C16" s="7" t="s">
@@ -1575,7 +1414,7 @@
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" ht="19.8" x14ac:dyDescent="0.4">
+    <row r="17" customFormat="false" ht="19.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4"/>
       <c r="B17" s="2" t="s">
         <v>43</v>
@@ -1586,7 +1425,7 @@
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4"/>
       <c r="B18" s="6" t="s">
         <v>45</v>
@@ -1597,7 +1436,7 @@
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4"/>
       <c r="B19" s="6" t="s">
         <v>47</v>
@@ -1608,7 +1447,7 @@
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4"/>
       <c r="B20" s="14"/>
       <c r="C20" s="7" t="s">
@@ -1617,7 +1456,7 @@
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" ht="16.8" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="21" customFormat="false" ht="16.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B21" s="2" t="s">
         <v>50</v>
       </c>
@@ -1625,322 +1464,331 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C22" s="7" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C23" s="7" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C24" s="12" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C25" s="12" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C26" s="12" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C27" s="12" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C28" s="7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C29" s="7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C30" s="7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C31" s="7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C32" s="7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C33" s="7" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C34" s="12" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C35" s="7" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C36" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C37" s="7" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C38" s="12" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="39" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C39" s="12" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="40" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C40" s="12" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="41" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C41" s="7" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="42" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C42" s="7" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="43" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C43" s="7" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="44" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C44" s="7" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="45" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C45" s="7" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="46" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C46" s="7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="47" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C47" s="7" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="48" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C48" s="7" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="49" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C49" s="7" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="50" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C50" s="7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="51" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C51" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="52" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C52" s="7" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="53" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C53" s="7" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="54" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C54" s="7" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="55" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C55" s="7" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="56" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C56" s="7" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="57" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C57" s="7" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="58" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C58" s="7" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="59" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C59" s="7" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="60" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C60" s="7" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="61" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C61" s="7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="62" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C62" s="7" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="63" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C63" s="7" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="64" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C64" s="7" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="65" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C65" s="7" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="66" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C66" s="7" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="67" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C67" s="7" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="68" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C68" s="7" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="69" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C69" s="12" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="70" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C70" s="7" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="71" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C71" s="7" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="72" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C72" s="7" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="73" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C73" s="7" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="74" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C74" s="7" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="75" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C75" s="7" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="76" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C76" s="7" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="77" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C77" s="7" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="78" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C78" s="7" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="79" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C79" s="7" t="s">
         <v>109</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <tabColor rgb="00FFFFFF"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D16" activeCellId="1" sqref="A22 D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="57.5546875" style="16"/>
-    <col min="2" max="2" width="14.33203125" style="17"/>
-    <col min="3" max="3" width="27" style="17"/>
-    <col min="4" max="4" width="46.33203125" style="17"/>
-    <col min="5" max="5" width="12.5546875" style="17"/>
-    <col min="6" max="6" width="9.44140625" style="17"/>
-    <col min="7" max="1025" width="8.5546875"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="16" width="57.5612244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="17" width="14.3367346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="17" width="27"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="17" width="46.3316326530612"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="17" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="17" width="9.43877551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.55612244897959"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="21" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" s="21" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="18" t="s">
         <v>110</v>
       </c>
@@ -1958,189 +1806,189 @@
       </c>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
         <v>115</v>
       </c>
       <c r="B2" s="23"/>
-      <c r="C2"/>
+      <c r="C2" s="0"/>
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="15" t="s">
         <v>116</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>118</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="24" t="s">
         <v>119</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="0" t="s">
         <v>121</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="15" t="s">
         <v>122</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="0" t="s">
         <v>123</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="15" t="s">
         <v>124</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="0" t="s">
         <v>125</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="25" t="s">
         <v>126</v>
       </c>
       <c r="B7" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="0" t="s">
         <v>128</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="25" t="s">
         <v>129</v>
       </c>
       <c r="B8" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="0" t="s">
         <v>130</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="24" t="s">
         <v>131</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="0" t="s">
         <v>132</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="27" t="s">
         <v>133</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="0" t="s">
         <v>134</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="27" t="s">
         <v>135</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="0" t="s">
         <v>136</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="15" t="s">
         <v>137</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="0" t="s">
         <v>138</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="24" t="s">
         <v>139</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="0" t="s">
         <v>138</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="15" t="s">
         <v>140</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="0" t="s">
         <v>141</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="17" t="s">
-        <v>212</v>
+        <v>142</v>
       </c>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="22" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -2148,7 +1996,7 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="15" t="s">
         <v>13</v>
       </c>
@@ -2156,38 +2004,48 @@
         <v>120</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
     </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <tabColor rgb="00FFFFFF"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A42" activeCellId="1" sqref="A22 A42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="57.5546875" style="16"/>
-    <col min="2" max="2" width="14.33203125" style="17"/>
-    <col min="3" max="3" width="38.21875" style="17"/>
-    <col min="4" max="4" width="78" style="17"/>
-    <col min="5" max="5" width="21.5546875" style="17"/>
-    <col min="6" max="6" width="9.44140625" style="17"/>
-    <col min="7" max="1025" width="8.5546875"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="16" width="57.5612244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="17" width="14.3367346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="17" width="38.219387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="17" width="78"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="17" width="21.5561224489796"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="17" width="9.43877551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.55612244897959"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="21" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" s="21" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="18" t="s">
         <v>110</v>
       </c>
@@ -2205,9 +2063,9 @@
       </c>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
@@ -2215,106 +2073,118 @@
       <c r="E2" s="23"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="15" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C3" t="s">
-        <v>146</v>
+      <c r="C3" s="17" t="s">
+        <v>147</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="15" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C4" t="s">
-        <v>148</v>
+      <c r="C4" s="17" t="s">
+        <v>149</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="24" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C5" t="s">
-        <v>152</v>
+      <c r="C5" s="17" t="s">
+        <v>153</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="15" t="s">
-        <v>153</v>
+    <row r="6" customFormat="false" ht="14.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="24" t="s">
+        <v>154</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="C6" t="s">
-        <v>154</v>
+        <v>120</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>155</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="15" t="s">
-        <v>155</v>
+    <row r="7" customFormat="false" ht="14.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="24" t="s">
+        <v>156</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="C7" t="s">
-        <v>156</v>
+        <v>120</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>157</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <tabColor rgb="00FFFFFF"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="A22 B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="57.5546875" style="16"/>
-    <col min="2" max="2" width="14.33203125" style="17"/>
-    <col min="3" max="3" width="7.6640625" style="17"/>
-    <col min="4" max="4" width="46.33203125" style="17"/>
-    <col min="5" max="5" width="12.5546875" style="17"/>
-    <col min="6" max="6" width="9.44140625" style="17"/>
-    <col min="7" max="1025" width="8.5546875"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="16" width="57.5612244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="17" width="14.3367346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="17" width="7.66836734693878"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="17" width="46.3316326530612"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="17" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="17" width="9.43877551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.55612244897959"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="21" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" s="21" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="18" t="s">
         <v>110</v>
       </c>
@@ -2332,7 +2202,7 @@
       </c>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
         <v>13</v>
       </c>
@@ -2342,45 +2212,54 @@
       <c r="E2" s="23"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="B3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B3" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="C3" t="s">
-        <v>146</v>
-      </c>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3"/>
-    </row>
+      <c r="C3" s="17" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <tabColor rgb="00FFFFFF"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="55.109375"/>
-    <col min="2" max="2" width="14.33203125"/>
-    <col min="3" max="3" width="38.21875"/>
-    <col min="4" max="4" width="52.44140625"/>
-    <col min="5" max="5" width="10.6640625"/>
-    <col min="6" max="1025" width="8.5546875"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.1020408163265"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3367346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.219387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="52.4387755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.55612244897959"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="21" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" s="21" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="18" t="s">
         <v>110</v>
       </c>
@@ -2398,494 +2277,518 @@
       </c>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:6" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="28" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="4" customFormat="false" ht="14.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="29" t="s">
         <v>139</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="0" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="B5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="C5" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C5" s="0" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="C6" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="C6" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="29" t="s">
-        <v>158</v>
-      </c>
-      <c r="B7" t="s">
+        <v>159</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="C7" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="C7" s="0" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="29" t="s">
-        <v>151</v>
-      </c>
-      <c r="B8" t="s">
+        <v>152</v>
+      </c>
+      <c r="B8" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="C8" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="C8" s="0" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
-        <v>159</v>
-      </c>
-      <c r="B9" t="s">
+        <v>160</v>
+      </c>
+      <c r="B9" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="C9" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C9" s="0" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="C10" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="C10" s="0" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="29" t="s">
-        <v>162</v>
-      </c>
-      <c r="B11" t="s">
+        <v>163</v>
+      </c>
+      <c r="B11" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="C11" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="C11" s="0" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="29" t="s">
-        <v>164</v>
-      </c>
-      <c r="B12" t="s">
+        <v>165</v>
+      </c>
+      <c r="B12" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="C12" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="C12" s="0" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="29" t="s">
-        <v>166</v>
-      </c>
-      <c r="B13" t="s">
+        <v>167</v>
+      </c>
+      <c r="B13" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="C13" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="C13" s="0" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="30" t="s">
-        <v>168</v>
-      </c>
-      <c r="B14" t="s">
+        <v>169</v>
+      </c>
+      <c r="B14" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="C14" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="C14" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="29" t="s">
-        <v>170</v>
-      </c>
-      <c r="B15" t="s">
+        <v>171</v>
+      </c>
+      <c r="B15" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="C15" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="C15" s="0" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="B16" t="s">
+        <v>173</v>
+      </c>
+      <c r="B16" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="C16" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="C16" s="0" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="30" t="s">
-        <v>153</v>
-      </c>
-      <c r="B17" t="s">
+        <v>154</v>
+      </c>
+      <c r="B17" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="C17" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="C17" s="0" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="29" t="s">
-        <v>174</v>
-      </c>
-      <c r="B18" t="s">
+        <v>175</v>
+      </c>
+      <c r="B18" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="C18" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="C18" s="0" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="29" t="s">
-        <v>176</v>
-      </c>
-      <c r="B19" t="s">
+        <v>177</v>
+      </c>
+      <c r="B19" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="C19" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="C19" s="0" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="30" t="s">
-        <v>178</v>
-      </c>
-      <c r="B20" t="s">
+        <v>179</v>
+      </c>
+      <c r="B20" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="C20" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="C20" s="0" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="30" t="s">
-        <v>180</v>
-      </c>
-      <c r="B21" t="s">
+        <v>181</v>
+      </c>
+      <c r="B21" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="C21" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A22" s="30" t="s">
+      <c r="C21" s="0" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="B22" t="s">
-        <v>127</v>
-      </c>
-      <c r="C22" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B22" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="29" t="s">
-        <v>182</v>
-      </c>
-      <c r="B23" t="s">
+        <v>183</v>
+      </c>
+      <c r="B23" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="C23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C23" s="0" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="28" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="15" t="s">
-        <v>185</v>
-      </c>
-      <c r="B25" t="s">
+        <v>186</v>
+      </c>
+      <c r="B25" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="C25" t="s">
-        <v>186</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="C25" s="0" t="s">
         <v>187</v>
       </c>
-    </row>
+      <c r="D25" s="0" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <tabColor rgb="00FFFFFF"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A10" activeCellId="1" sqref="A22 A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="47.88671875"/>
-    <col min="2" max="2" width="27.88671875"/>
-    <col min="3" max="1025" width="9.88671875"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.8877551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.8877551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.89285714285714"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="21" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" s="21" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="18" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>189</v>
-      </c>
-      <c r="C1"/>
-      <c r="D1"/>
+        <v>190</v>
+      </c>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="31" t="str">
-        <f>HYPERLINK("http://www.w3.org/2001/XMLSchema-instance","http://www.w3.org/2001/XMLSchema-instance")</f>
+        <f aca="false">HYPERLINK("http://www.w3.org/2001/XMLSchema-instance","http://www.w3.org/2001/XMLSchema-instance")</f>
         <v>http://www.w3.org/2001/XMLSchema-instance</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="31" t="str">
-        <f>HYPERLINK("http://stix.mitre.org/stix-1","http://stix.mitre.org/stix-1")</f>
+        <f aca="false">HYPERLINK("http://stix.mitre.org/stix-1","http://stix.mitre.org/stix-1")</f>
         <v>http://stix.mitre.org/stix-1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="31" t="str">
-        <f>HYPERLINK("http://stix.mitre.org/common-1","http://stix.mitre.org/common-1")</f>
+        <f aca="false">HYPERLINK("http://stix.mitre.org/common-1","http://stix.mitre.org/common-1")</f>
         <v>http://stix.mitre.org/common-1</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="31" t="str">
-        <f>HYPERLINK("http://stix.mitre.org/default_vocabularies-1","http://stix.mitre.org/default_vocabularies-1")</f>
+        <f aca="false">HYPERLINK("http://stix.mitre.org/default_vocabularies-1","http://stix.mitre.org/default_vocabularies-1")</f>
         <v>http://stix.mitre.org/default_vocabularies-1</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="32" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="32" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="32" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="32" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A6" r:id="rId1"/>
-    <hyperlink ref="A7" r:id="rId2"/>
-    <hyperlink ref="A8" r:id="rId3"/>
-    <hyperlink ref="A9" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId1" display="http://stix.mitre.org/TTP-1"/>
+    <hyperlink ref="A7" r:id="rId2" display="http://stix.mitre.org/Incident-1"/>
+    <hyperlink ref="A8" r:id="rId3" display="http://cybox.mitre.org/cybox-2"/>
+    <hyperlink ref="A9" r:id="rId4" display="http://stix.mitre.org/Indicator-2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <tabColor rgb="00FFFFFF"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="1" sqref="A22 B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="33.88671875"/>
-    <col min="2" max="2" width="36.44140625"/>
-    <col min="3" max="3" width="25.6640625"/>
-    <col min="4" max="1025" width="17.109375"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.8928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.4489795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.6683673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="17.1071428571429"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="21" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" s="21" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="18" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>204</v>
-      </c>
-      <c r="D1"/>
+        <v>205</v>
+      </c>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="B2" t="s">
-        <v>205</v>
+      <c r="B2" s="0" t="s">
+        <v>206</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>144</v>
-      </c>
-      <c r="B3" t="s">
         <v>207</v>
       </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>208</v>
+      </c>
       <c r="C3" s="32" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
-        <v>208</v>
+      <c r="B4" s="0" t="s">
+        <v>209</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>142</v>
-      </c>
-      <c r="B5" t="s">
-        <v>209</v>
+        <v>195</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>210</v>
       </c>
       <c r="C5" s="32" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>184</v>
-      </c>
-      <c r="B6" t="s">
-        <v>210</v>
+        <v>207</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>211</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>157</v>
-      </c>
-      <c r="B7" t="s">
-        <v>211</v>
+        <v>199</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>212</v>
       </c>
       <c r="C7" s="32" t="s">
-        <v>200</v>
-      </c>
-    </row>
+        <v>201</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
-    <hyperlink ref="C6" r:id="rId5"/>
-    <hyperlink ref="C7" r:id="rId6"/>
+    <hyperlink ref="C2" r:id="rId1" display="http://stix.mitre.org/stix-1"/>
+    <hyperlink ref="C3" r:id="rId2" display="http://stix.mitre.org/stix-1"/>
+    <hyperlink ref="C4" r:id="rId3" display="http://stix.mitre.org/TTP-1"/>
+    <hyperlink ref="C5" r:id="rId4" display="http://stix.mitre.org/stix-1"/>
+    <hyperlink ref="C6" r:id="rId5" display="http://cybox.mitre.org/cybox-2"/>
+    <hyperlink ref="C7" r:id="rId6" display="http://stix.mitre.org/Indicator-2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added better Profile support for optional fields which have value constraints. Fixes #30. * If an optional field is has value constraints and is an   attribute, it gets its own schematron rule context. * Fixed an issue where rule contexts were not being fired because   a superset context was fired instead. This was accomplished by   wrapping each schematron rule inside its own pattern. TBH, i'm   not sure why this seems to work.
</commit_message>
<xml_diff>
--- a/examples/Example_Profile.xlsx
+++ b/examples/Example_Profile.xlsx
@@ -1,27 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\stix-validator\examples\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="480" firstSheet="0" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="480" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="STIX Package" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="STIX Header" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="TTP" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Indicator" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Namespaces" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="Instance Mapping" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Overview" sheetId="1" r:id="rId1"/>
+    <sheet name="STIX Package" sheetId="2" r:id="rId2"/>
+    <sheet name="STIX Header" sheetId="3" r:id="rId3"/>
+    <sheet name="TTP" sheetId="4" r:id="rId4"/>
+    <sheet name="Email Message Object" sheetId="11" r:id="rId5"/>
+    <sheet name="Domain Object" sheetId="10" r:id="rId6"/>
+    <sheet name="Indicator" sheetId="5" r:id="rId7"/>
+    <sheet name="Namespaces" sheetId="6" r:id="rId8"/>
+    <sheet name="Instance Mapping" sheetId="7" r:id="rId9"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="232">
   <si>
     <t>Profile Information</t>
   </si>
@@ -660,38 +666,76 @@
   </si>
   <si>
     <t>stix:Indicator</t>
+  </si>
+  <si>
+    <t>@apply_condition</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>DomainNameObj:Value</t>
+  </si>
+  <si>
+    <t>DomainNameObject:Value</t>
+  </si>
+  <si>
+    <t>http://cybox.mitre.org/objects#DomainNameObject-1</t>
+  </si>
+  <si>
+    <t>DomainNameObj</t>
+  </si>
+  <si>
+    <t>@is_case_sensitive</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>DomainNameObject</t>
+  </si>
+  <si>
+    <t>cybox:Properties[@xsi:type="DomainNameObj:DomainNameObjectType"]</t>
+  </si>
+  <si>
+    <t>www.example.com</t>
+  </si>
+  <si>
+    <t>EmailMessageObject:Header</t>
+  </si>
+  <si>
+    <t>From</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Free Face Enlargement Pills!</t>
+  </si>
+  <si>
+    <t>EmailMessageObj:Header</t>
+  </si>
+  <si>
+    <t>http://cybox.mitre.org/objects#EmailMessageObject-2</t>
+  </si>
+  <si>
+    <t>EmailMessageObj</t>
+  </si>
+  <si>
+    <t>ANY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-  </numFmts>
-  <fonts count="22">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -701,7 +745,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="15"/>
       <color rgb="FF1F497D"/>
       <name val="Calibri"/>
@@ -709,7 +753,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="15"/>
       <color rgb="FF1F497D"/>
       <name val="Calibri"/>
@@ -724,7 +768,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -746,14 +790,14 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="1"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -768,7 +812,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -803,7 +847,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
@@ -811,7 +855,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
@@ -819,15 +863,22 @@
       <charset val="1"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -864,16 +915,21 @@
         <bgColor rgb="FF003300"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -882,7 +938,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top style="thick">
@@ -891,21 +947,25 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
-      <top style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="medium">
         <color rgb="FFDDDDDD"/>
       </left>
@@ -916,21 +976,27 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="medium">
         <color rgb="FFDDDDDD"/>
       </left>
@@ -942,183 +1008,74 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="36">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="33">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="6" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="6" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="8" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="8" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="19" fillId="7" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="8">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="TableStyleLight1" xfId="21" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
+  <cellStyles count="4">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="TableStyleLight1" xfId="3"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1177,33 +1134,309 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF1F497D"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
-    <pageSetUpPr fitToPage="false"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
   <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C24" activeCellId="1" sqref="A22 C24"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C24" activeCellId="1" sqref="A22 C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="67.6683673469388"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.5561224489796"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.1020408163265"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.55612244897959"/>
+    <col min="1" max="1" width="67.7109375"/>
+    <col min="2" max="2" width="34.5703125"/>
+    <col min="3" max="3" width="38.140625"/>
+    <col min="4" max="4" width="43.7109375"/>
+    <col min="5" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1219,7 +1452,7 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -1235,7 +1468,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>8</v>
       </c>
@@ -1251,7 +1484,7 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>12</v>
       </c>
@@ -1267,7 +1500,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
@@ -1281,7 +1514,7 @@
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>19</v>
       </c>
@@ -1297,7 +1530,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>23</v>
       </c>
@@ -1313,7 +1546,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
       <c r="B8" s="7" t="s">
         <v>27</v>
@@ -1327,7 +1560,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
       <c r="B9" s="7" t="s">
         <v>30</v>
@@ -1341,7 +1574,7 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="14"/>
       <c r="C10" s="12" t="s">
@@ -1353,7 +1586,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" customFormat="false" ht="19.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:6" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="2" t="s">
         <v>34</v>
@@ -1365,7 +1598,7 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="14"/>
       <c r="C12" s="7" t="s">
@@ -1374,7 +1607,7 @@
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" customFormat="false" ht="19.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:6" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="2" t="s">
         <v>37</v>
@@ -1385,7 +1618,7 @@
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="14"/>
       <c r="C14" s="6" t="s">
@@ -1394,7 +1627,7 @@
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" customFormat="false" ht="19.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:6" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="2" t="s">
         <v>40</v>
@@ -1405,7 +1638,7 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="14"/>
       <c r="C16" s="7" t="s">
@@ -1414,7 +1647,7 @@
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" customFormat="false" ht="19.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:6" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="2" t="s">
         <v>43</v>
@@ -1425,7 +1658,7 @@
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="6" t="s">
         <v>45</v>
@@ -1436,7 +1669,7 @@
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="6" t="s">
         <v>47</v>
@@ -1447,7 +1680,7 @@
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="14"/>
       <c r="C20" s="7" t="s">
@@ -1456,7 +1689,7 @@
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" customFormat="false" ht="16.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
         <v>50</v>
       </c>
@@ -1464,331 +1697,325 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="7" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="7" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" s="12" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="12" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C26" s="12" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C27" s="12" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C28" s="7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C29" s="7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C30" s="7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C31" s="7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C32" s="7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="33" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C33" s="7" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="34" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C34" s="12" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="35" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C35" s="7" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="36" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C36" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="37" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C37" s="7" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="38" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C38" s="12" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="39" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C39" s="12" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="40" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C40" s="12" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="41" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C41" s="7" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="42" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C42" s="7" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="43" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C43" s="7" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="44" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C44" s="7" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="45" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C45" s="7" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="46" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C46" s="7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="47" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C47" s="7" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="48" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C48" s="7" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="49" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C49" s="7" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="50" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C50" s="7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="51" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C51" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="52" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C52" s="7" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="53" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C53" s="7" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="54" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C54" s="7" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="55" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C55" s="7" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="56" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C56" s="7" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="57" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C57" s="7" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="58" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C58" s="7" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="59" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C59" s="7" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="60" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C60" s="7" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="61" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C61" s="7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="62" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C62" s="7" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="63" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C63" s="7" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="64" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C64" s="7" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="65" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C65" s="7" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="66" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C66" s="7" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="67" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C67" s="7" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="68" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C68" s="7" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="69" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C69" s="12" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="70" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C70" s="7" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="71" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C71" s="7" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="72" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C72" s="7" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="73" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C73" s="7" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="74" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C74" s="7" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="75" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C75" s="7" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="76" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C76" s="7" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="77" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C77" s="7" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="78" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C78" s="7" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="79" spans="3:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C79" s="7" t="s">
         <v>109</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
-    <pageSetUpPr fitToPage="false"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="1" sqref="A22 D16"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="16" width="57.5612244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="17" width="14.3367346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="17" width="27"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="17" width="46.3316326530612"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="17" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="17" width="9.43877551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.55612244897959"/>
+    <col min="1" max="1" width="57.5703125" style="16"/>
+    <col min="2" max="2" width="14.28515625" style="17"/>
+    <col min="3" max="3" width="27" style="17"/>
+    <col min="4" max="4" width="46.28515625" style="17"/>
+    <col min="5" max="5" width="12.5703125" style="17"/>
+    <col min="6" max="6" width="9.42578125" style="17"/>
+    <col min="7" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" s="21" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" s="21" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>110</v>
       </c>
@@ -1806,178 +2033,178 @@
       </c>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>115</v>
       </c>
       <c r="B2" s="23"/>
-      <c r="C2" s="0"/>
+      <c r="C2"/>
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>116</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" t="s">
         <v>118</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
         <v>119</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" t="s">
         <v>121</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>122</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" t="s">
         <v>123</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>124</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" t="s">
         <v>125</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
         <v>126</v>
       </c>
       <c r="B7" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" t="s">
         <v>128</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
         <v>129</v>
       </c>
       <c r="B8" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" t="s">
         <v>130</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
         <v>131</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" t="s">
         <v>132</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="27" t="s">
         <v>133</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" t="s">
         <v>134</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="27" t="s">
         <v>135</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" t="s">
         <v>136</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>137</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" t="s">
         <v>138</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="24" t="s">
         <v>139</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" t="s">
         <v>138</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>140</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" t="s">
         <v>141</v>
       </c>
       <c r="D14" s="4"/>
@@ -1986,7 +2213,7 @@
       </c>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>143</v>
       </c>
@@ -1996,7 +2223,7 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>13</v>
       </c>
@@ -2010,42 +2237,35 @@
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
-    <pageSetUpPr fitToPage="false"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A42" activeCellId="1" sqref="A22 A42"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A42" activeCellId="1" sqref="A22 A42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="16" width="57.5612244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="17" width="14.3367346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="17" width="38.219387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="17" width="78"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="17" width="21.5561224489796"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="17" width="9.43877551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.55612244897959"/>
+    <col min="1" max="1" width="57.5703125" style="16"/>
+    <col min="2" max="2" width="14.28515625" style="17"/>
+    <col min="3" max="3" width="38.28515625" style="17"/>
+    <col min="4" max="4" width="78" style="17"/>
+    <col min="5" max="5" width="21.5703125" style="17"/>
+    <col min="6" max="6" width="9.42578125" style="17"/>
+    <col min="7" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" s="21" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" s="21" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>110</v>
       </c>
@@ -2063,7 +2283,7 @@
       </c>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>145</v>
       </c>
@@ -2073,7 +2293,7 @@
       <c r="E2" s="23"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>146</v>
       </c>
@@ -2087,7 +2307,7 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>148</v>
       </c>
@@ -2105,7 +2325,7 @@
       </c>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
         <v>152</v>
       </c>
@@ -2119,7 +2339,7 @@
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" customFormat="false" ht="14.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="24" t="s">
         <v>154</v>
       </c>
@@ -2133,7 +2353,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" customFormat="false" ht="14.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
         <v>156</v>
       </c>
@@ -2147,44 +2367,35 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
-    <pageSetUpPr fitToPage="false"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="A22 B3"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B3" activeCellId="1" sqref="A22 B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="16" width="57.5612244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="17" width="14.3367346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="17" width="7.66836734693878"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="17" width="46.3316326530612"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="17" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="17" width="9.43877551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.55612244897959"/>
+    <col min="1" max="1" width="57.5703125" style="16"/>
+    <col min="2" max="2" width="14.28515625" style="17"/>
+    <col min="3" max="3" width="7.7109375" style="17"/>
+    <col min="4" max="4" width="46.28515625" style="17"/>
+    <col min="5" max="5" width="12.5703125" style="17"/>
+    <col min="6" max="6" width="9.42578125" style="17"/>
+    <col min="7" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" s="21" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" s="21" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>110</v>
       </c>
@@ -2202,7 +2413,7 @@
       </c>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>13</v>
       </c>
@@ -2212,7 +2423,7 @@
       <c r="E2" s="23"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>146</v>
       </c>
@@ -2223,43 +2434,32 @@
         <v>147</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
-    <pageSetUpPr fitToPage="false"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
+    <sheetView showFormulas="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.1020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3367346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.219387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="52.4387755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.55612244897959"/>
+    <col min="1" max="1" width="45.85546875" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="21" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" s="21" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="18" t="s">
         <v>110</v>
       </c>
@@ -2277,423 +2477,586 @@
       </c>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="28" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="B3" s="0" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
+        <v>225</v>
+      </c>
+      <c r="B3" t="s">
         <v>117</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="29" t="s">
-        <v>139</v>
-      </c>
-      <c r="B4" s="0" t="s">
+      <c r="E3" s="34"/>
+    </row>
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
+        <v>226</v>
+      </c>
+      <c r="B4" t="s">
         <v>120</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="29" t="s">
-        <v>159</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="29" t="s">
-        <v>152</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="29" t="s">
-        <v>160</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="29" t="s">
-        <v>163</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="29" t="s">
-        <v>165</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="29" t="s">
-        <v>167</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="30" t="s">
-        <v>169</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="29" t="s">
-        <v>171</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="29" t="s">
-        <v>173</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="30" t="s">
-        <v>154</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="29" t="s">
-        <v>175</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="29" t="s">
-        <v>177</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="30" t="s">
-        <v>179</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="30" t="s">
-        <v>181</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="29" t="s">
-        <v>183</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="28" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="15" t="s">
-        <v>186</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>187</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="E4" t="s">
+        <v>227</v>
+      </c>
+    </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
-    <pageSetUpPr fitToPage="false"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="1" sqref="A22 A10"/>
+    <sheetView showFormulas="1" tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.8877551020408"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.8877551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.89285714285714"/>
+    <col min="1" max="1" width="81" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="21" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" s="21" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="18" t="s">
-        <v>189</v>
-      </c>
-      <c r="B1" s="19" t="s">
-        <v>190</v>
-      </c>
-      <c r="E1" s="4"/>
-    </row>
-    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="31" t="str">
-        <f aca="false">HYPERLINK("http://www.w3.org/2001/XMLSchema-instance","http://www.w3.org/2001/XMLSchema-instance")</f>
-        <v>http://www.w3.org/2001/XMLSchema-instance</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-    </row>
-    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="31" t="str">
-        <f aca="false">HYPERLINK("http://stix.mitre.org/stix-1","http://stix.mitre.org/stix-1")</f>
-        <v>http://stix.mitre.org/stix-1</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="31" t="str">
-        <f aca="false">HYPERLINK("http://stix.mitre.org/common-1","http://stix.mitre.org/common-1")</f>
-        <v>http://stix.mitre.org/common-1</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="31" t="str">
-        <f aca="false">HYPERLINK("http://stix.mitre.org/default_vocabularies-1","http://stix.mitre.org/default_vocabularies-1")</f>
-        <v>http://stix.mitre.org/default_vocabularies-1</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="32" t="s">
-        <v>195</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-    </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="32" t="s">
-        <v>197</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-    </row>
-    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="32" t="s">
-        <v>199</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-    </row>
-    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="32" t="s">
-        <v>201</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
+        <v>110</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="28" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="33" t="s">
+        <v>214</v>
+      </c>
+      <c r="B3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E3" s="34" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" s="28" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
+        <v>213</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E5" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="33" t="s">
+        <v>219</v>
+      </c>
+      <c r="B6" t="s">
+        <v>120</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>220</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A6" r:id="rId1" display="http://stix.mitre.org/TTP-1"/>
-    <hyperlink ref="A7" r:id="rId2" display="http://stix.mitre.org/Incident-1"/>
-    <hyperlink ref="A8" r:id="rId3" display="http://cybox.mitre.org/cybox-2"/>
-    <hyperlink ref="A9" r:id="rId4" display="http://stix.mitre.org/Indicator-2"/>
+    <hyperlink ref="E3" r:id="rId1"/>
   </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
-    <pageSetUpPr fitToPage="false"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="1" sqref="A22 B8"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.8928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.4489795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.6683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="17.1071428571429"/>
+    <col min="1" max="1" width="55.140625"/>
+    <col min="2" max="2" width="14.28515625"/>
+    <col min="3" max="3" width="38.28515625"/>
+    <col min="4" max="4" width="52.42578125"/>
+    <col min="5" max="5" width="10.7109375"/>
+    <col min="6" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" s="21" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" s="21" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A2" s="28" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="B4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="B5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="B6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="B7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A8" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="B8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A9" s="29" t="s">
+        <v>160</v>
+      </c>
+      <c r="B9" t="s">
+        <v>120</v>
+      </c>
+      <c r="C9" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A11" s="29" t="s">
+        <v>163</v>
+      </c>
+      <c r="B11" t="s">
+        <v>120</v>
+      </c>
+      <c r="C11" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A12" s="29" t="s">
+        <v>165</v>
+      </c>
+      <c r="B12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C12" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A13" s="29" t="s">
+        <v>167</v>
+      </c>
+      <c r="B13" t="s">
+        <v>120</v>
+      </c>
+      <c r="C13" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A14" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="B14" t="s">
+        <v>127</v>
+      </c>
+      <c r="C14" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A15" s="29" t="s">
+        <v>171</v>
+      </c>
+      <c r="B15" t="s">
+        <v>120</v>
+      </c>
+      <c r="C15" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A16" s="29" t="s">
+        <v>173</v>
+      </c>
+      <c r="B16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C16" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A17" s="30" t="s">
+        <v>154</v>
+      </c>
+      <c r="B17" t="s">
+        <v>127</v>
+      </c>
+      <c r="C17" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A18" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="B18" t="s">
+        <v>120</v>
+      </c>
+      <c r="C18" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A19" s="29" t="s">
+        <v>177</v>
+      </c>
+      <c r="B19" t="s">
+        <v>120</v>
+      </c>
+      <c r="C19" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A20" s="30" t="s">
+        <v>179</v>
+      </c>
+      <c r="B20" t="s">
+        <v>127</v>
+      </c>
+      <c r="C20" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A21" s="30" t="s">
+        <v>181</v>
+      </c>
+      <c r="B21" t="s">
+        <v>127</v>
+      </c>
+      <c r="C21" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="B22" t="s">
+        <v>117</v>
+      </c>
+      <c r="C22" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="29" t="s">
+        <v>183</v>
+      </c>
+      <c r="B23" t="s">
+        <v>120</v>
+      </c>
+      <c r="C23" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A24" s="28" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="B25" t="s">
+        <v>117</v>
+      </c>
+      <c r="C25" t="s">
+        <v>187</v>
+      </c>
+      <c r="D25" t="s">
+        <v>188</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="47.85546875"/>
+    <col min="2" max="2" width="27.85546875"/>
+    <col min="3" max="1025" width="9.85546875"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="21" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>190</v>
+      </c>
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="31" t="str">
+        <f>HYPERLINK("http://www.w3.org/2001/XMLSchema-instance","http://www.w3.org/2001/XMLSchema-instance")</f>
+        <v>http://www.w3.org/2001/XMLSchema-instance</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="31" t="str">
+        <f>HYPERLINK("http://stix.mitre.org/stix-1","http://stix.mitre.org/stix-1")</f>
+        <v>http://stix.mitre.org/stix-1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="31" t="str">
+        <f>HYPERLINK("http://stix.mitre.org/common-1","http://stix.mitre.org/common-1")</f>
+        <v>http://stix.mitre.org/common-1</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="31" t="str">
+        <f>HYPERLINK("http://stix.mitre.org/default_vocabularies-1","http://stix.mitre.org/default_vocabularies-1")</f>
+        <v>http://stix.mitre.org/default_vocabularies-1</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="32" t="s">
+        <v>195</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="32" t="s">
+        <v>197</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="32" t="s">
+        <v>199</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="34" t="s">
+        <v>217</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>229</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>230</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A6" r:id="rId1"/>
+    <hyperlink ref="A7" r:id="rId2"/>
+    <hyperlink ref="A8" r:id="rId3"/>
+    <hyperlink ref="A9" r:id="rId4"/>
+    <hyperlink ref="A10" r:id="rId5" location="DomainNameObject-1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
+  </sheetPr>
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="33.85546875"/>
+    <col min="2" max="2" width="78.85546875" customWidth="1"/>
+    <col min="3" max="3" width="45.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="1025" width="17.140625"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="21" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>203</v>
       </c>
@@ -2705,90 +3068,115 @@
       </c>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>115</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>206</v>
       </c>
       <c r="C2" s="32" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>145</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>208</v>
       </c>
       <c r="C3" s="32" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>209</v>
       </c>
       <c r="C4" s="32" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>143</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>210</v>
       </c>
       <c r="C5" s="32" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>185</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>211</v>
       </c>
       <c r="C6" s="32" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>158</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" t="s">
         <v>212</v>
       </c>
       <c r="C7" s="32" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>216</v>
+      </c>
+      <c r="B8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C8" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>221</v>
+      </c>
+      <c r="B9" t="s">
+        <v>222</v>
+      </c>
+      <c r="C9" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>224</v>
+      </c>
+      <c r="B10" t="s">
+        <v>228</v>
+      </c>
+      <c r="C10" t="s">
+        <v>229</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="http://stix.mitre.org/stix-1"/>
-    <hyperlink ref="C3" r:id="rId2" display="http://stix.mitre.org/stix-1"/>
-    <hyperlink ref="C4" r:id="rId3" display="http://stix.mitre.org/TTP-1"/>
-    <hyperlink ref="C5" r:id="rId4" display="http://stix.mitre.org/stix-1"/>
-    <hyperlink ref="C6" r:id="rId5" display="http://cybox.mitre.org/cybox-2"/>
-    <hyperlink ref="C7" r:id="rId6" display="http://stix.mitre.org/Indicator-2"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C6" r:id="rId5"/>
+    <hyperlink ref="C7" r:id="rId6"/>
   </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>